<commit_message>
Lab1 protocol and code changed
</commit_message>
<xml_diff>
--- a/cp1/zaritskyi_fb-01_svirshchuk_fb-01_cp1/Bigram_Crossed_Frequency_with_space.xlsx
+++ b/cp1/zaritskyi_fb-01_svirshchuk_fb-01_cp1/Bigram_Crossed_Frequency_with_space.xlsx
@@ -588,88 +588,88 @@
         <v>0</v>
       </c>
       <c r="B2">
-        <v>0.00900768567394168</v>
+        <v>0</v>
       </c>
       <c r="C2">
-        <v>0.002714151685446499</v>
+        <v>0.002604962385658203</v>
       </c>
       <c r="D2">
-        <v>0.006021550212753859</v>
+        <v>0.005695333500937941</v>
       </c>
       <c r="E2">
-        <v>0.01662512675202093</v>
+        <v>0.0160358931714015</v>
       </c>
       <c r="F2">
-        <v>0.006669762416959657</v>
+        <v>0.005959310758281924</v>
       </c>
       <c r="G2">
-        <v>0.007932070393570948</v>
+        <v>0.007599257382660658</v>
       </c>
       <c r="H2">
-        <v>0.006275528093933909</v>
+        <v>0.00605503877468139</v>
       </c>
       <c r="I2">
         <v>0</v>
       </c>
       <c r="J2">
-        <v>0.002832611518086447</v>
+        <v>0.002709392949003075</v>
       </c>
       <c r="K2">
-        <v>0.004018157523147051</v>
+        <v>0.003835889303602855</v>
       </c>
       <c r="L2">
-        <v>0.02584319708873115</v>
+        <v>0.02548879305343364</v>
       </c>
       <c r="M2">
         <v>0</v>
       </c>
       <c r="N2">
-        <v>0.007876157352564892</v>
+        <v>0.007519967510491404</v>
       </c>
       <c r="O2">
-        <v>0.001931369111361719</v>
+        <v>0.001846873851747278</v>
       </c>
       <c r="P2">
-        <v>0.006312487561717573</v>
+        <v>0.006044402328414783</v>
       </c>
       <c r="Q2">
-        <v>0.01259275404895708</v>
+        <v>0.01216809452899882</v>
       </c>
       <c r="R2">
-        <v>0.01015911524720198</v>
+        <v>0.009704306793788316</v>
       </c>
       <c r="S2">
-        <v>0.01438670975445646</v>
+        <v>0.01345993927556131</v>
       </c>
       <c r="T2">
-        <v>0.00307995564863866</v>
+        <v>0.002891179485196001</v>
       </c>
       <c r="U2">
-        <v>0.01942551719562931</v>
+        <v>0.01850451565491501</v>
       </c>
       <c r="V2">
-        <v>0.008579334919115627</v>
+        <v>0.0082364772089965</v>
       </c>
       <c r="W2">
-        <v>0.003319718349901915</v>
+        <v>0.003153222843218782</v>
       </c>
       <c r="X2">
-        <v>0.0006633750627837113</v>
+        <v>0.0005869384439846062</v>
       </c>
       <c r="Y2">
-        <v>0.001409198169084827</v>
+        <v>0.001295712545204897</v>
       </c>
       <c r="Z2">
-        <v>0.000978952056936534</v>
+        <v>0.0009350403218008471</v>
       </c>
       <c r="AA2">
-        <v>0.003508306403464713</v>
+        <v>0.003345645825678315</v>
       </c>
       <c r="AB2">
-        <v>0.0005705025539939917</v>
+        <v>0.0005308553636697674</v>
       </c>
       <c r="AC2">
-        <v>1.705821590015258E-05</v>
+        <v>1.643814423021138E-05</v>
       </c>
       <c r="AD2">
         <v>0</v>
@@ -681,13 +681,13 @@
         <v>0</v>
       </c>
       <c r="AG2">
-        <v>0.0008007884686460515</v>
+        <v>0.0007880639733895454</v>
       </c>
       <c r="AH2">
-        <v>0.0001118260820121113</v>
+        <v>0.0001024966640236709</v>
       </c>
       <c r="AI2">
-        <v>0.00163190265444793</v>
+        <v>0.001613838983542517</v>
       </c>
     </row>
     <row r="3" spans="1:35">
@@ -695,88 +695,88 @@
         <v>1</v>
       </c>
       <c r="B3">
-        <v>0.01699093071521308</v>
+        <v>0.0163240441702605</v>
       </c>
       <c r="C3">
-        <v>0.001015911524720198</v>
+        <v>0.001049140381751726</v>
       </c>
       <c r="D3">
-        <v>0.0007761488234569422</v>
+        <v>0.0008470479026861862</v>
       </c>
       <c r="E3">
-        <v>0.004126192890514684</v>
+        <v>0.004296157342048773</v>
       </c>
       <c r="F3">
-        <v>0.0008055268619516495</v>
+        <v>0.0009098996306252297</v>
       </c>
       <c r="G3">
-        <v>0.001964537864500905</v>
+        <v>0.002053801079115821</v>
       </c>
       <c r="H3">
-        <v>0.0007211834611120061</v>
+        <v>0.00076582413119573</v>
       </c>
       <c r="I3">
         <v>0</v>
       </c>
       <c r="J3">
-        <v>0.0008737597255522598</v>
+        <v>0.0009137674292676323</v>
       </c>
       <c r="K3">
-        <v>0.003394584964130363</v>
+        <v>0.003488754375447214</v>
       </c>
       <c r="L3">
-        <v>0.001426256384984979</v>
+        <v>0.001538416910015665</v>
       </c>
       <c r="M3">
-        <v>0.0009533647330863051</v>
+        <v>0.0009727513585642731</v>
       </c>
       <c r="N3">
-        <v>0.002744477402602326</v>
+        <v>0.002848633700129571</v>
       </c>
       <c r="O3">
-        <v>0.007084845670530037</v>
+        <v>0.007242452957899012</v>
       </c>
       <c r="P3">
-        <v>0.004164100036959468</v>
+        <v>0.004294223442727571</v>
       </c>
       <c r="Q3">
-        <v>0.003064792790060746</v>
+        <v>0.003186099131679205</v>
       </c>
       <c r="R3">
-        <v>0.0002975710995915505</v>
+        <v>0.0003558374751010462</v>
       </c>
       <c r="S3">
-        <v>0.0005278570142436103</v>
+        <v>0.0006188477827844283</v>
       </c>
       <c r="T3">
-        <v>0.003530103012670464</v>
+        <v>0.003628962076234311</v>
       </c>
       <c r="U3">
-        <v>0.002269690393381412</v>
+        <v>0.002420275000483475</v>
       </c>
       <c r="V3">
-        <v>0.002631703641929095</v>
+        <v>0.002757740432033108</v>
       </c>
       <c r="W3">
-        <v>0.0003999203949924659</v>
+        <v>0.0004244909010036938</v>
       </c>
       <c r="X3">
-        <v>0.0004292984334871732</v>
+        <v>0.0004428629445551065</v>
       </c>
       <c r="Y3">
-        <v>0.0009751613422920556</v>
+        <v>0.001000792898721692</v>
       </c>
       <c r="Z3">
-        <v>3.506411046142474E-05</v>
+        <v>4.351273472703011E-05</v>
       </c>
       <c r="AA3">
-        <v>0.000475734687882033</v>
+        <v>0.0004979790752093446</v>
       </c>
       <c r="AB3">
-        <v>0.001131528321376788</v>
+        <v>0.001158405693399602</v>
       </c>
       <c r="AC3">
-        <v>0.000135518048540101</v>
+        <v>0.0001382738014658957</v>
       </c>
       <c r="AD3">
         <v>0</v>
@@ -788,13 +788,13 @@
         <v>0</v>
       </c>
       <c r="AG3">
-        <v>9.476786611195875E-07</v>
+        <v>3.867798642402676E-06</v>
       </c>
       <c r="AH3">
-        <v>0.0004908975464599463</v>
+        <v>0.0005018468738517473</v>
       </c>
       <c r="AI3">
-        <v>0.0004890021891377072</v>
+        <v>0.0005018468738517473</v>
       </c>
     </row>
     <row r="4" spans="1:35">
@@ -802,106 +802,106 @@
         <v>2</v>
       </c>
       <c r="B4">
-        <v>0.0003932866443646288</v>
+        <v>0.0003732425689918583</v>
       </c>
       <c r="C4">
-        <v>0.000422664682859336</v>
+        <v>0.0004312595486278985</v>
       </c>
       <c r="D4">
-        <v>4.359321841150103E-05</v>
+        <v>4.834748303003345E-05</v>
       </c>
       <c r="E4">
-        <v>1.231982259455464E-05</v>
+        <v>1.353729524840937E-05</v>
       </c>
       <c r="F4">
-        <v>0</v>
+        <v>9.669496606006691E-07</v>
       </c>
       <c r="G4">
-        <v>7.5814292889567E-06</v>
+        <v>8.702546945406021E-06</v>
       </c>
       <c r="H4">
-        <v>0.00179206034817714</v>
+        <v>0.001829468757856466</v>
       </c>
       <c r="I4">
         <v>0</v>
       </c>
       <c r="J4">
-        <v>2.843035983358763E-06</v>
+        <v>2.900848981802008E-06</v>
       </c>
       <c r="K4">
         <v>0</v>
       </c>
       <c r="L4">
-        <v>0.0006880147079728206</v>
+        <v>0.0007020054535960858</v>
       </c>
       <c r="M4">
         <v>0</v>
       </c>
       <c r="N4">
-        <v>2.369196652798969E-05</v>
+        <v>2.417374151501673E-05</v>
       </c>
       <c r="O4">
-        <v>0.0009325158025416741</v>
+        <v>0.0009514784660310584</v>
       </c>
       <c r="P4">
-        <v>2.463964518910928E-05</v>
+        <v>2.51406911756174E-05</v>
       </c>
       <c r="Q4">
-        <v>0.0002416580585854948</v>
+        <v>0.0002475391131137713</v>
       </c>
       <c r="R4">
-        <v>0.003190834051989651</v>
+        <v>0.003264422054187859</v>
       </c>
       <c r="S4">
         <v>0</v>
       </c>
       <c r="T4">
-        <v>0.001384558523895718</v>
+        <v>0.001413680403798178</v>
       </c>
       <c r="U4">
-        <v>3.695946778366391E-05</v>
+        <v>3.77110367634261E-05</v>
       </c>
       <c r="V4">
-        <v>8.529107950076288E-06</v>
+        <v>1.353729524840937E-05</v>
       </c>
       <c r="W4">
-        <v>0.001503966035196785</v>
+        <v>0.001536483010694463</v>
       </c>
       <c r="X4">
         <v>0</v>
       </c>
       <c r="Y4">
-        <v>2.843035983358763E-06</v>
+        <v>2.900848981802008E-06</v>
       </c>
       <c r="Z4">
         <v>0</v>
       </c>
       <c r="AA4">
-        <v>1.895357322239175E-06</v>
+        <v>1.933899321201338E-06</v>
       </c>
       <c r="AB4">
-        <v>5.686071966717526E-06</v>
+        <v>5.801697963604015E-06</v>
       </c>
       <c r="AC4">
-        <v>0.0001412041205068186</v>
+        <v>0.0001440754994294997</v>
       </c>
       <c r="AD4">
-        <v>8.055268619516495E-05</v>
+        <v>8.219072115105688E-05</v>
       </c>
       <c r="AE4">
-        <v>0.002455435410960851</v>
+        <v>0.002505366570616334</v>
       </c>
       <c r="AF4">
-        <v>5.022696903933814E-05</v>
+        <v>5.124833201183547E-05</v>
       </c>
       <c r="AG4">
-        <v>0</v>
+        <v>9.669496606006691E-07</v>
       </c>
       <c r="AH4">
-        <v>0</v>
+        <v>1.933899321201338E-06</v>
       </c>
       <c r="AI4">
-        <v>0.0007088636385174515</v>
+        <v>0.0007232783461293005</v>
       </c>
     </row>
     <row r="5" spans="1:35">
@@ -909,85 +909,85 @@
         <v>3</v>
       </c>
       <c r="B5">
-        <v>0.007174875143336397</v>
+        <v>0.006766713724883483</v>
       </c>
       <c r="C5">
-        <v>0.004781986524009438</v>
+        <v>0.004886963584675782</v>
       </c>
       <c r="D5">
-        <v>4.738393305597937E-06</v>
+        <v>1.353729524840937E-05</v>
       </c>
       <c r="E5">
-        <v>7.676197155068659E-05</v>
+        <v>0.0001092653116478756</v>
       </c>
       <c r="F5">
-        <v>1.895357322239175E-06</v>
+        <v>4.157883540582877E-05</v>
       </c>
       <c r="G5">
-        <v>8.908179414524124E-05</v>
+        <v>0.000114100059950879</v>
       </c>
       <c r="H5">
-        <v>0.005130732271301447</v>
+        <v>0.005252470556382834</v>
       </c>
       <c r="I5">
-        <v>9.476786611195875E-07</v>
+        <v>9.669496606006691E-07</v>
       </c>
       <c r="J5">
-        <v>9.476786611195875E-07</v>
+        <v>1.933899321201338E-05</v>
       </c>
       <c r="K5">
-        <v>0.0005136418343268164</v>
+        <v>0.0005550291051847841</v>
       </c>
       <c r="L5">
-        <v>0.003321613707224154</v>
+        <v>0.00345394418766559</v>
       </c>
       <c r="M5">
         <v>0</v>
       </c>
       <c r="N5">
-        <v>4.359321841150103E-05</v>
+        <v>8.12237714904562E-05</v>
       </c>
       <c r="O5">
-        <v>0.0006472645255446783</v>
+        <v>0.0006671952658144617</v>
       </c>
       <c r="P5">
-        <v>0.0001099307246898722</v>
+        <v>0.0001276373551992883</v>
       </c>
       <c r="Q5">
-        <v>0.0004491996853706845</v>
+        <v>0.0004805739813185325</v>
       </c>
       <c r="R5">
-        <v>0.009386757138389514</v>
+        <v>0.009596975381461641</v>
       </c>
       <c r="S5">
-        <v>5.022696903933814E-05</v>
+        <v>0.000117000908932681</v>
       </c>
       <c r="T5">
-        <v>0.0009258820519138371</v>
+        <v>0.0009669496606006692</v>
       </c>
       <c r="U5">
-        <v>0.002743529723941206</v>
+        <v>0.002852501498771974</v>
       </c>
       <c r="V5">
-        <v>8.813411548412165E-05</v>
+        <v>0.0001150670096114796</v>
       </c>
       <c r="W5">
-        <v>0.0009884288435477299</v>
+        <v>0.001016264093291303</v>
       </c>
       <c r="X5">
-        <v>8.529107950076288E-06</v>
+        <v>1.353729524840937E-05</v>
       </c>
       <c r="Y5">
-        <v>0.0001099307246898722</v>
+        <v>0.000122802606896285</v>
       </c>
       <c r="Z5">
-        <v>3.695946778366391E-05</v>
+        <v>4.06118857452281E-05</v>
       </c>
       <c r="AA5">
-        <v>0.0002065939481240701</v>
+        <v>0.0002214314722775532</v>
       </c>
       <c r="AB5">
-        <v>0.0004037111096369443</v>
+        <v>0.0004186892030400897</v>
       </c>
       <c r="AC5">
         <v>0</v>
@@ -996,19 +996,19 @@
         <v>0</v>
       </c>
       <c r="AE5">
-        <v>0.002818396338169653</v>
+        <v>0.00287570829062639</v>
       </c>
       <c r="AF5">
-        <v>0.0003421119966641711</v>
+        <v>0.0003490688274768416</v>
       </c>
       <c r="AG5">
-        <v>0</v>
+        <v>9.669496606006691E-07</v>
       </c>
       <c r="AH5">
-        <v>0</v>
+        <v>9.669496606006691E-07</v>
       </c>
       <c r="AI5">
-        <v>0.0009476786611195875</v>
+        <v>0.0009669496606006692</v>
       </c>
     </row>
     <row r="6" spans="1:35">
@@ -1016,25 +1016,25 @@
         <v>4</v>
       </c>
       <c r="B6">
-        <v>0.001050975635181623</v>
+        <v>0.001013363244309501</v>
       </c>
       <c r="C6">
-        <v>0.001122051534765592</v>
+        <v>0.001146802297472394</v>
       </c>
       <c r="D6">
-        <v>2.843035983358763E-06</v>
+        <v>5.801697963604015E-06</v>
       </c>
       <c r="E6">
-        <v>3.79071464447835E-06</v>
+        <v>1.063644626660736E-05</v>
       </c>
       <c r="F6">
-        <v>7.5814292889567E-06</v>
+        <v>1.25703455878087E-05</v>
       </c>
       <c r="G6">
-        <v>0.001038655812587068</v>
+        <v>0.001061710727339535</v>
       </c>
       <c r="H6">
-        <v>0.0003496934259531278</v>
+        <v>0.0003587383240828482</v>
       </c>
       <c r="I6">
         <v>0</v>
@@ -1043,58 +1043,58 @@
         <v>0</v>
       </c>
       <c r="K6">
-        <v>9.476786611195875E-07</v>
+        <v>1.933899321201338E-06</v>
       </c>
       <c r="L6">
-        <v>0.0008491200803631505</v>
+        <v>0.0008721885938618036</v>
       </c>
       <c r="M6">
         <v>0</v>
       </c>
       <c r="N6">
-        <v>1.895357322239175E-06</v>
+        <v>2.900848981802008E-06</v>
       </c>
       <c r="O6">
-        <v>0.0007666720368457463</v>
+        <v>0.0007822622754259413</v>
       </c>
       <c r="P6">
-        <v>0</v>
+        <v>1.933899321201338E-06</v>
       </c>
       <c r="Q6">
-        <v>0.0004406705774206082</v>
+        <v>0.0004525324411611131</v>
       </c>
       <c r="R6">
-        <v>0.01239374153012197</v>
+        <v>0.01265060240963855</v>
       </c>
       <c r="S6">
-        <v>0</v>
+        <v>4.834748303003346E-06</v>
       </c>
       <c r="T6">
-        <v>0.0005458629088048824</v>
+        <v>0.0005579299541665861</v>
       </c>
       <c r="U6">
-        <v>6.633750627837113E-06</v>
+        <v>1.063644626660736E-05</v>
       </c>
       <c r="V6">
-        <v>1.895357322239175E-06</v>
+        <v>9.669496606006692E-06</v>
       </c>
       <c r="W6">
-        <v>0.000362960927208802</v>
+        <v>0.000371308669670657</v>
       </c>
       <c r="X6">
         <v>0</v>
       </c>
       <c r="Y6">
-        <v>0</v>
+        <v>9.669496606006691E-07</v>
       </c>
       <c r="Z6">
         <v>0</v>
       </c>
       <c r="AA6">
-        <v>4.738393305597937E-06</v>
+        <v>6.768647624204684E-06</v>
       </c>
       <c r="AB6">
-        <v>2.843035983358763E-06</v>
+        <v>2.900848981802008E-06</v>
       </c>
       <c r="AC6">
         <v>0</v>
@@ -1123,106 +1123,106 @@
         <v>5</v>
       </c>
       <c r="B7">
-        <v>0.002352138436898816</v>
+        <v>0.002236554564969348</v>
       </c>
       <c r="C7">
-        <v>0.005644374105628264</v>
+        <v>0.005760119128198186</v>
       </c>
       <c r="D7">
-        <v>1.326750125567423E-05</v>
+        <v>1.353729524840937E-05</v>
       </c>
       <c r="E7">
-        <v>0.0007098113171785711</v>
+        <v>0.0007290800440929046</v>
       </c>
       <c r="F7">
-        <v>7.5814292889567E-06</v>
+        <v>4.641358370883212E-05</v>
       </c>
       <c r="G7">
-        <v>3.885482510590309E-05</v>
+        <v>4.447968438763078E-05</v>
       </c>
       <c r="H7">
-        <v>0.006032922356687295</v>
+        <v>0.006159469338026262</v>
       </c>
       <c r="I7">
         <v>0</v>
       </c>
       <c r="J7">
-        <v>0</v>
+        <v>5.801697963604015E-06</v>
       </c>
       <c r="K7">
-        <v>2.653500251134845E-05</v>
+        <v>2.80415401574194E-05</v>
       </c>
       <c r="L7">
-        <v>0.002514191487950266</v>
+        <v>0.002581755593803787</v>
       </c>
       <c r="M7">
         <v>0</v>
       </c>
       <c r="N7">
-        <v>3.506411046142474E-05</v>
+        <v>4.544663404823145E-05</v>
       </c>
       <c r="O7">
-        <v>0.0008898702627912927</v>
+        <v>0.0009128004796070317</v>
       </c>
       <c r="P7">
-        <v>7.297125690620824E-05</v>
+        <v>8.315767081165754E-05</v>
       </c>
       <c r="Q7">
-        <v>0.001816699993366249</v>
+        <v>0.001867179794619892</v>
       </c>
       <c r="R7">
-        <v>0.003760388927322523</v>
+        <v>0.003846525749869462</v>
       </c>
       <c r="S7">
-        <v>5.686071966717526E-06</v>
+        <v>1.353729524840937E-05</v>
       </c>
       <c r="T7">
-        <v>0.0005145895129879361</v>
+        <v>0.000528921464348566</v>
       </c>
       <c r="U7">
-        <v>0.0002094369841074288</v>
+        <v>0.0002282001199017579</v>
       </c>
       <c r="V7">
-        <v>7.202357824508865E-05</v>
+        <v>7.83229225086542E-05</v>
       </c>
       <c r="W7">
-        <v>0.002015712512201363</v>
+        <v>0.002059602777079425</v>
       </c>
       <c r="X7">
-        <v>1.895357322239175E-06</v>
+        <v>6.768647624204684E-06</v>
       </c>
       <c r="Y7">
-        <v>2.463964518910928E-05</v>
+        <v>2.51406911756174E-05</v>
       </c>
       <c r="Z7">
-        <v>0.0005231186209380123</v>
+        <v>0.0005337562126515693</v>
       </c>
       <c r="AA7">
-        <v>2.843035983358763E-06</v>
+        <v>4.834748303003346E-06</v>
       </c>
       <c r="AB7">
-        <v>8.43434008396433E-05</v>
+        <v>8.605851979345956E-05</v>
       </c>
       <c r="AC7">
         <v>0</v>
       </c>
       <c r="AD7">
-        <v>2.843035983358763E-06</v>
+        <v>2.900848981802008E-06</v>
       </c>
       <c r="AE7">
-        <v>0.0006737995280560267</v>
+        <v>0.0006875012086870757</v>
       </c>
       <c r="AF7">
-        <v>0.001675495872859431</v>
+        <v>0.001709566999941983</v>
       </c>
       <c r="AG7">
         <v>0</v>
       </c>
       <c r="AH7">
-        <v>5.686071966717526E-06</v>
+        <v>5.801697963604015E-06</v>
       </c>
       <c r="AI7">
-        <v>0.0002283905573298206</v>
+        <v>0.0002330348682047612</v>
       </c>
     </row>
     <row r="8" spans="1:35">
@@ -1230,88 +1230,88 @@
         <v>6</v>
       </c>
       <c r="B8">
-        <v>0.01549738914528861</v>
+        <v>0.01469956874045137</v>
       </c>
       <c r="C8">
-        <v>6.82328636006103E-05</v>
+        <v>7.83229225086542E-05</v>
       </c>
       <c r="D8">
-        <v>0.002373935046104567</v>
+        <v>0.00248602757740432</v>
       </c>
       <c r="E8">
-        <v>0.002388150226021361</v>
+        <v>0.002534375060434354</v>
       </c>
       <c r="F8">
-        <v>0.005426408013570759</v>
+        <v>0.005623779226053492</v>
       </c>
       <c r="G8">
-        <v>0.002694250433562988</v>
+        <v>0.002802220116420739</v>
       </c>
       <c r="H8">
-        <v>0.001322959410922944</v>
+        <v>0.001383704964319558</v>
       </c>
       <c r="I8">
         <v>0</v>
       </c>
       <c r="J8">
-        <v>0.0008671259749244226</v>
+        <v>0.000894428436055619</v>
       </c>
       <c r="K8">
-        <v>0.0005752409472995897</v>
+        <v>0.0006198147324450289</v>
       </c>
       <c r="L8">
-        <v>0.0001620530510514495</v>
+        <v>0.0002282001199017579</v>
       </c>
       <c r="M8">
-        <v>0.002686669004274031</v>
+        <v>0.002741302287802897</v>
       </c>
       <c r="N8">
-        <v>0.0008187943632073237</v>
+        <v>0.0008818580904678102</v>
       </c>
       <c r="O8">
-        <v>0.005850020375091214</v>
+        <v>0.005985418399118141</v>
       </c>
       <c r="P8">
-        <v>0.005424512656248519</v>
+        <v>0.005567696145738652</v>
       </c>
       <c r="Q8">
-        <v>0.006694402062148767</v>
+        <v>0.006874045137210157</v>
       </c>
       <c r="R8">
-        <v>0.0001345703698789814</v>
+        <v>0.0002098280763503452</v>
       </c>
       <c r="S8">
-        <v>0.0004245600401815752</v>
+        <v>0.0005850045446634048</v>
       </c>
       <c r="T8">
-        <v>0.004345106661233309</v>
+        <v>0.004461505734011487</v>
       </c>
       <c r="U8">
-        <v>0.004921295287194019</v>
+        <v>0.005142238295074359</v>
       </c>
       <c r="V8">
-        <v>0.004478729352451171</v>
+        <v>0.004608482082422789</v>
       </c>
       <c r="W8">
-        <v>4.927929037821855E-05</v>
+        <v>8.12237714904562E-05</v>
       </c>
       <c r="X8">
-        <v>0.000530700050226969</v>
+        <v>0.0005501943568817807</v>
       </c>
       <c r="Y8">
-        <v>0.0008775504401967381</v>
+        <v>0.0009302055734978438</v>
       </c>
       <c r="Z8">
-        <v>0.0003705423564977587</v>
+        <v>0.0003838790152584657</v>
       </c>
       <c r="AA8">
-        <v>0.000887027226807934</v>
+        <v>0.000926337774855441</v>
       </c>
       <c r="AB8">
-        <v>0.0008728120468911401</v>
+        <v>0.0008963623353768203</v>
       </c>
       <c r="AC8">
-        <v>0.0003127339581694639</v>
+        <v>0.0003190933879982208</v>
       </c>
       <c r="AD8">
         <v>0</v>
@@ -1323,13 +1323,13 @@
         <v>0</v>
       </c>
       <c r="AG8">
-        <v>6.633750627837113E-06</v>
+        <v>6.768647624204684E-06</v>
       </c>
       <c r="AH8">
-        <v>0.0006785379213616247</v>
+        <v>0.0006923359569900791</v>
       </c>
       <c r="AI8">
-        <v>0.0003269491380862577</v>
+        <v>0.0003384323812102342</v>
       </c>
     </row>
     <row r="9" spans="1:35">
@@ -1337,7 +1337,7 @@
         <v>7</v>
       </c>
       <c r="B9">
-        <v>4.359321841150103E-05</v>
+        <v>4.351273472703011E-05</v>
       </c>
       <c r="C9">
         <v>0</v>
@@ -1364,7 +1364,7 @@
         <v>0</v>
       </c>
       <c r="K9">
-        <v>0</v>
+        <v>9.669496606006691E-07</v>
       </c>
       <c r="L9">
         <v>0</v>
@@ -1376,7 +1376,7 @@
         <v>0</v>
       </c>
       <c r="O9">
-        <v>9.476786611195875E-07</v>
+        <v>9.669496606006691E-07</v>
       </c>
       <c r="P9">
         <v>0</v>
@@ -1391,7 +1391,7 @@
         <v>0</v>
       </c>
       <c r="T9">
-        <v>9.476786611195875E-07</v>
+        <v>9.669496606006691E-07</v>
       </c>
       <c r="U9">
         <v>0</v>
@@ -1444,70 +1444,70 @@
         <v>8</v>
       </c>
       <c r="B10">
-        <v>6.159911297277319E-05</v>
+        <v>5.898392929664082E-05</v>
       </c>
       <c r="C10">
-        <v>0.0006235725590166886</v>
+        <v>0.0006362528766752402</v>
       </c>
       <c r="D10">
-        <v>3.980250376702268E-05</v>
+        <v>4.06118857452281E-05</v>
       </c>
       <c r="E10">
-        <v>1.042446527231546E-05</v>
+        <v>1.063644626660736E-05</v>
       </c>
       <c r="F10">
-        <v>3.506411046142474E-05</v>
+        <v>3.577713744222476E-05</v>
       </c>
       <c r="G10">
-        <v>0.0008775504401967381</v>
+        <v>0.0008953953857162196</v>
       </c>
       <c r="H10">
-        <v>0.003379422105552449</v>
+        <v>0.003449109439362587</v>
       </c>
       <c r="I10">
         <v>0</v>
       </c>
       <c r="J10">
-        <v>0.0002122800200907876</v>
+        <v>0.0002165967239745499</v>
       </c>
       <c r="K10">
         <v>0</v>
       </c>
       <c r="L10">
-        <v>0.001869769998388946</v>
+        <v>0.00190779168036512</v>
       </c>
       <c r="M10">
         <v>0</v>
       </c>
       <c r="N10">
-        <v>1.51628585779134E-05</v>
+        <v>1.547119456961071E-05</v>
       </c>
       <c r="O10">
         <v>0</v>
       </c>
       <c r="P10">
-        <v>9.476786611195875E-07</v>
+        <v>9.669496606006691E-07</v>
       </c>
       <c r="Q10">
-        <v>0.000524066299599132</v>
+        <v>0.0005347231623121701</v>
       </c>
       <c r="R10">
-        <v>1.137214393343505E-05</v>
+        <v>1.160339592720803E-05</v>
       </c>
       <c r="S10">
-        <v>0</v>
+        <v>1.933899321201338E-06</v>
       </c>
       <c r="T10">
-        <v>5.686071966717525E-05</v>
+        <v>5.801697963604015E-05</v>
       </c>
       <c r="U10">
-        <v>9.476786611195875E-07</v>
+        <v>1.933899321201338E-06</v>
       </c>
       <c r="V10">
         <v>0</v>
       </c>
       <c r="W10">
-        <v>0.0001857450175794392</v>
+        <v>0.0001895221334777311</v>
       </c>
       <c r="X10">
         <v>0</v>
@@ -1519,7 +1519,7 @@
         <v>0</v>
       </c>
       <c r="AA10">
-        <v>3.980250376702268E-05</v>
+        <v>4.06118857452281E-05</v>
       </c>
       <c r="AB10">
         <v>0</v>
@@ -1534,7 +1534,7 @@
         <v>0</v>
       </c>
       <c r="AF10">
-        <v>3.316875313918556E-05</v>
+        <v>3.384323812102342E-05</v>
       </c>
       <c r="AG10">
         <v>0</v>
@@ -1551,70 +1551,70 @@
         <v>9</v>
       </c>
       <c r="B11">
-        <v>0.001841339638555359</v>
+        <v>0.001743410238063007</v>
       </c>
       <c r="C11">
-        <v>0.004654997583419414</v>
+        <v>0.004749656732870487</v>
       </c>
       <c r="D11">
-        <v>0.0001573146577458515</v>
+        <v>0.0001624475429809124</v>
       </c>
       <c r="E11">
-        <v>0.000822585077851802</v>
+        <v>0.0008470479026861862</v>
       </c>
       <c r="F11">
-        <v>0.0001393087631845794</v>
+        <v>0.0001508441470537044</v>
       </c>
       <c r="G11">
-        <v>0.000346850389969769</v>
+        <v>0.0003606722234040496</v>
       </c>
       <c r="H11">
-        <v>0.00140256441845699</v>
+        <v>0.001434953296331393</v>
       </c>
       <c r="I11">
         <v>0</v>
       </c>
       <c r="J11">
-        <v>2.843035983358763E-06</v>
+        <v>4.834748303003346E-06</v>
       </c>
       <c r="K11">
-        <v>7.202357824508865E-05</v>
+        <v>8.219072115105688E-05</v>
       </c>
       <c r="L11">
-        <v>0.0002786175263691588</v>
+        <v>0.0002968535458044054</v>
       </c>
       <c r="M11">
         <v>0</v>
       </c>
       <c r="N11">
-        <v>3.601178912254433E-05</v>
+        <v>5.02813823512348E-05</v>
       </c>
       <c r="O11">
-        <v>0.0004311937908094123</v>
+        <v>0.0004409290452339051</v>
       </c>
       <c r="P11">
-        <v>0.0001175121539788289</v>
+        <v>0.000125703455878087</v>
       </c>
       <c r="Q11">
-        <v>0.0006861193506505814</v>
+        <v>0.0007126418998626931</v>
       </c>
       <c r="R11">
-        <v>0.0004738393305597938</v>
+        <v>0.0004844417799609353</v>
       </c>
       <c r="S11">
-        <v>2.843035983358763E-06</v>
+        <v>1.643814423021138E-05</v>
       </c>
       <c r="T11">
-        <v>0.00137982013059012</v>
+        <v>0.001409812605155776</v>
       </c>
       <c r="U11">
-        <v>9.476786611195875E-07</v>
+        <v>2.610764083621807E-05</v>
       </c>
       <c r="V11">
-        <v>6.633750627837113E-06</v>
+        <v>1.063644626660736E-05</v>
       </c>
       <c r="W11">
-        <v>0.0001127737606732309</v>
+        <v>0.0001160339592720803</v>
       </c>
       <c r="X11">
         <v>0</v>
@@ -1623,10 +1623,10 @@
         <v>0</v>
       </c>
       <c r="Z11">
-        <v>2.843035983358763E-06</v>
+        <v>2.900848981802008E-06</v>
       </c>
       <c r="AA11">
-        <v>2.843035983358763E-06</v>
+        <v>6.768647624204684E-06</v>
       </c>
       <c r="AB11">
         <v>0</v>
@@ -1635,22 +1635,22 @@
         <v>0</v>
       </c>
       <c r="AD11">
-        <v>1.895357322239175E-06</v>
+        <v>1.933899321201338E-06</v>
       </c>
       <c r="AE11">
-        <v>0.0001734251949848845</v>
+        <v>0.0001769517878899224</v>
       </c>
       <c r="AF11">
-        <v>0.0002757744903858</v>
+        <v>0.0002813823512347947</v>
       </c>
       <c r="AG11">
         <v>0</v>
       </c>
       <c r="AH11">
-        <v>5.686071966717526E-06</v>
+        <v>5.801697963604015E-06</v>
       </c>
       <c r="AI11">
-        <v>0.0004605718293041196</v>
+        <v>0.0004699375350519252</v>
       </c>
     </row>
     <row r="12" spans="1:35">
@@ -1658,88 +1658,88 @@
         <v>10</v>
       </c>
       <c r="B12">
-        <v>0.03001014016167398</v>
+        <v>0.02869229727900366</v>
       </c>
       <c r="C12">
-        <v>0.0006368400602723629</v>
+        <v>0.0006816995107234718</v>
       </c>
       <c r="D12">
-        <v>0.0008690213322466618</v>
+        <v>0.0009543793150128604</v>
       </c>
       <c r="E12">
-        <v>0.001321064053600705</v>
+        <v>0.001535516061033863</v>
       </c>
       <c r="F12">
-        <v>0.0002397627012632557</v>
+        <v>0.0003190933879982208</v>
       </c>
       <c r="G12">
-        <v>0.001775949810938107</v>
+        <v>0.001885551838171305</v>
       </c>
       <c r="H12">
-        <v>0.001988229831028895</v>
+        <v>0.002093446015200449</v>
       </c>
       <c r="I12">
         <v>0</v>
       </c>
       <c r="J12">
-        <v>0.0001819543029349608</v>
+        <v>0.0002156297743139492</v>
       </c>
       <c r="K12">
-        <v>0.00356232408714853</v>
+        <v>0.003673441760621942</v>
       </c>
       <c r="L12">
-        <v>0.0008955563347580102</v>
+        <v>0.001033669187182115</v>
       </c>
       <c r="M12">
-        <v>0.0008339572217852371</v>
+        <v>0.0008509157013285888</v>
       </c>
       <c r="N12">
-        <v>0.001878299106339023</v>
+        <v>0.001992883250497979</v>
       </c>
       <c r="O12">
-        <v>0.006454639360885511</v>
+        <v>0.00660329923224197</v>
       </c>
       <c r="P12">
-        <v>0.003367102282957895</v>
+        <v>0.003477150979520006</v>
       </c>
       <c r="Q12">
-        <v>0.00335478246036334</v>
+        <v>0.003547738304743855</v>
       </c>
       <c r="R12">
-        <v>0.0007117066745008102</v>
+        <v>0.0008721885938618036</v>
       </c>
       <c r="S12">
-        <v>0.0004615195079652391</v>
+        <v>0.0007590554835715253</v>
       </c>
       <c r="T12">
-        <v>0.0007524568569289526</v>
+        <v>0.0008248080604923708</v>
       </c>
       <c r="U12">
-        <v>0.003727220174183338</v>
+        <v>0.004075692819431821</v>
       </c>
       <c r="V12">
-        <v>0.003527259976687105</v>
+        <v>0.003672474810961341</v>
       </c>
       <c r="W12">
-        <v>0.0001639484083736886</v>
+        <v>0.0002117619756715465</v>
       </c>
       <c r="X12">
-        <v>0.0003231584234417793</v>
+        <v>0.0003461679784950395</v>
       </c>
       <c r="Y12">
-        <v>0.003217369054501</v>
+        <v>0.003309868688236091</v>
       </c>
       <c r="Z12">
-        <v>0.0007069682811952123</v>
+        <v>0.0007290800440929046</v>
       </c>
       <c r="AA12">
-        <v>0.0002340766292965381</v>
+        <v>0.0002678450559863853</v>
       </c>
       <c r="AB12">
-        <v>0.0007136020318230494</v>
+        <v>0.0007339147923959079</v>
       </c>
       <c r="AC12">
-        <v>0.0003013618142360289</v>
+        <v>0.0003084569417316135</v>
       </c>
       <c r="AD12">
         <v>0</v>
@@ -1751,13 +1751,13 @@
         <v>0</v>
       </c>
       <c r="AG12">
-        <v>3.79071464447835E-06</v>
+        <v>5.801697963604015E-06</v>
       </c>
       <c r="AH12">
-        <v>0.0003165246728139422</v>
+        <v>0.0003239281363012242</v>
       </c>
       <c r="AI12">
-        <v>0.001305901195022792</v>
+        <v>0.001340192229592527</v>
       </c>
     </row>
     <row r="13" spans="1:35">
@@ -1765,85 +1765,85 @@
         <v>11</v>
       </c>
       <c r="B13">
-        <v>0.006807175822821998</v>
+        <v>0.006540447504302926</v>
       </c>
       <c r="C13">
-        <v>0</v>
+        <v>3.867798642402676E-06</v>
       </c>
       <c r="D13">
-        <v>0</v>
+        <v>1.353729524840937E-05</v>
       </c>
       <c r="E13">
-        <v>4.738393305597937E-06</v>
+        <v>2.80415401574194E-05</v>
       </c>
       <c r="F13">
-        <v>4.738393305597937E-06</v>
+        <v>3.867798642402677E-05</v>
       </c>
       <c r="G13">
-        <v>0.0005780839832829484</v>
+        <v>0.0006140130344814249</v>
       </c>
       <c r="H13">
-        <v>9.476786611195875E-07</v>
+        <v>8.702546945406021E-06</v>
       </c>
       <c r="I13">
         <v>0</v>
       </c>
       <c r="J13">
-        <v>0</v>
+        <v>8.702546945406021E-06</v>
       </c>
       <c r="K13">
-        <v>0</v>
+        <v>1.25703455878087E-05</v>
       </c>
       <c r="L13">
-        <v>9.476786611195875E-07</v>
+        <v>3.674408710282543E-05</v>
       </c>
       <c r="M13">
         <v>0</v>
       </c>
       <c r="N13">
-        <v>5.686071966717526E-06</v>
+        <v>2.610764083621807E-05</v>
       </c>
       <c r="O13">
-        <v>7.5814292889567E-06</v>
+        <v>1.25703455878087E-05</v>
       </c>
       <c r="P13">
-        <v>1.990125188351134E-05</v>
+        <v>3.674408710282543E-05</v>
       </c>
       <c r="Q13">
-        <v>0.0002028032334795917</v>
+        <v>0.0002301340192229592</v>
       </c>
       <c r="R13">
-        <v>9.476786611195875E-07</v>
+        <v>1.837204355141271E-05</v>
       </c>
       <c r="S13">
-        <v>0</v>
+        <v>3.867798642402677E-05</v>
       </c>
       <c r="T13">
-        <v>3.79071464447835E-06</v>
+        <v>1.547119456961071E-05</v>
       </c>
       <c r="U13">
-        <v>0.0003316875313918556</v>
+        <v>0.0003896807132220697</v>
       </c>
       <c r="V13">
-        <v>0.0004359321841150103</v>
+        <v>0.0004564002398035158</v>
       </c>
       <c r="W13">
-        <v>0</v>
+        <v>1.160339592720803E-05</v>
       </c>
       <c r="X13">
-        <v>0</v>
+        <v>2.900848981802008E-06</v>
       </c>
       <c r="Y13">
-        <v>0</v>
+        <v>6.768647624204684E-06</v>
       </c>
       <c r="Z13">
-        <v>5.401768368381649E-05</v>
+        <v>5.705002997543948E-05</v>
       </c>
       <c r="AA13">
-        <v>9.476786611195875E-07</v>
+        <v>8.702546945406021E-06</v>
       </c>
       <c r="AB13">
-        <v>0.0001260412619289052</v>
+        <v>0.000137306851805295</v>
       </c>
       <c r="AC13">
         <v>0</v>
@@ -1858,13 +1858,13 @@
         <v>0</v>
       </c>
       <c r="AG13">
-        <v>0</v>
+        <v>1.933899321201338E-06</v>
       </c>
       <c r="AH13">
         <v>0</v>
       </c>
       <c r="AI13">
-        <v>3.79071464447835E-06</v>
+        <v>8.702546945406021E-06</v>
       </c>
     </row>
     <row r="14" spans="1:35">
@@ -1872,85 +1872,85 @@
         <v>12</v>
       </c>
       <c r="B14">
-        <v>0.003946133944901962</v>
+        <v>0.003762401129397204</v>
       </c>
       <c r="C14">
-        <v>0.005489902483865771</v>
+        <v>0.005610241930805083</v>
       </c>
       <c r="D14">
-        <v>9.476786611195875E-07</v>
+        <v>7.735597284805353E-06</v>
       </c>
       <c r="E14">
-        <v>7.676197155068659E-05</v>
+        <v>9.476106673886557E-05</v>
       </c>
       <c r="F14">
-        <v>9.476786611195875E-07</v>
+        <v>2.707459049681873E-05</v>
       </c>
       <c r="G14">
-        <v>9.476786611195875E-07</v>
+        <v>8.702546945406021E-06</v>
       </c>
       <c r="H14">
-        <v>0.0003402166393419319</v>
+        <v>0.0003539035757798449</v>
       </c>
       <c r="I14">
         <v>0</v>
       </c>
       <c r="J14">
-        <v>8.244804351740412E-05</v>
+        <v>8.992631843586223E-05</v>
       </c>
       <c r="K14">
-        <v>0</v>
+        <v>4.834748303003346E-06</v>
       </c>
       <c r="L14">
-        <v>0.001819543029349608</v>
+        <v>0.001874915391904697</v>
       </c>
       <c r="M14">
         <v>0</v>
       </c>
       <c r="N14">
-        <v>4.454089707262062E-05</v>
+        <v>6.188477827844282E-05</v>
       </c>
       <c r="O14">
-        <v>0.0006804332786838639</v>
+        <v>0.0006952368059718811</v>
       </c>
       <c r="P14">
-        <v>9.476786611195875E-07</v>
+        <v>5.801697963604015E-06</v>
       </c>
       <c r="Q14">
-        <v>0.0001184598326399484</v>
+        <v>0.0001450424490901004</v>
       </c>
       <c r="R14">
-        <v>0.006636593663820471</v>
+        <v>0.006787019667756097</v>
       </c>
       <c r="S14">
-        <v>9.476786611195875E-07</v>
+        <v>2.707459049681873E-05</v>
       </c>
       <c r="T14">
-        <v>0.001262307976611291</v>
+        <v>0.001294745595544296</v>
       </c>
       <c r="U14">
-        <v>2.084893054463093E-05</v>
+        <v>5.801697963604015E-05</v>
       </c>
       <c r="V14">
-        <v>0.0004956359397655443</v>
+        <v>0.0005163511187607573</v>
       </c>
       <c r="W14">
-        <v>0.0009325158025416741</v>
+        <v>0.0009553462646734611</v>
       </c>
       <c r="X14">
-        <v>9.476786611195875E-07</v>
+        <v>3.867798642402676E-06</v>
       </c>
       <c r="Y14">
-        <v>1.705821590015258E-05</v>
+        <v>1.837204355141271E-05</v>
       </c>
       <c r="Z14">
-        <v>0</v>
+        <v>3.867798642402676E-06</v>
       </c>
       <c r="AA14">
-        <v>0</v>
+        <v>2.900848981802008E-06</v>
       </c>
       <c r="AB14">
-        <v>2.843035983358763E-06</v>
+        <v>3.867798642402676E-06</v>
       </c>
       <c r="AC14">
         <v>0</v>
@@ -1968,10 +1968,10 @@
         <v>0</v>
       </c>
       <c r="AH14">
-        <v>0</v>
+        <v>3.867798642402676E-06</v>
       </c>
       <c r="AI14">
-        <v>0</v>
+        <v>9.669496606006691E-07</v>
       </c>
     </row>
     <row r="15" spans="1:35">
@@ -1979,106 +1979,106 @@
         <v>13</v>
       </c>
       <c r="B15">
-        <v>0.008398328294841785</v>
+        <v>0.008219072115105688</v>
       </c>
       <c r="C15">
-        <v>0.005080505302262109</v>
+        <v>0.005200255274710399</v>
       </c>
       <c r="D15">
-        <v>7.676197155068659E-05</v>
+        <v>9.186021775706357E-05</v>
       </c>
       <c r="E15">
-        <v>2.084893054463093E-05</v>
+        <v>4.157883540582877E-05</v>
       </c>
       <c r="F15">
-        <v>6.82328636006103E-05</v>
+        <v>0.0001034636136842716</v>
       </c>
       <c r="G15">
-        <v>1.042446527231546E-05</v>
+        <v>2.417374151501673E-05</v>
       </c>
       <c r="H15">
-        <v>0.005259616569213711</v>
+        <v>0.005402347753775938</v>
       </c>
       <c r="I15">
         <v>0</v>
       </c>
       <c r="J15">
-        <v>0.0004833161171709897</v>
+        <v>0.0004960451758881432</v>
       </c>
       <c r="K15">
-        <v>4.738393305597937E-06</v>
+        <v>7.735597284805353E-06</v>
       </c>
       <c r="L15">
-        <v>0.007523620890628406</v>
+        <v>0.007708522694308534</v>
       </c>
       <c r="M15">
         <v>0</v>
       </c>
       <c r="N15">
-        <v>0.0001175121539788289</v>
+        <v>0.0001276373551992883</v>
       </c>
       <c r="O15">
-        <v>4.643625439485979E-05</v>
+        <v>5.221528167243614E-05</v>
       </c>
       <c r="P15">
-        <v>5.875607698941443E-05</v>
+        <v>7.638902318745286E-05</v>
       </c>
       <c r="Q15">
-        <v>0.0002615593104690062</v>
+        <v>0.0002852501498771974</v>
       </c>
       <c r="R15">
-        <v>0.004455037385923181</v>
+        <v>0.004564969347695759</v>
       </c>
       <c r="S15">
-        <v>2.937803849470721E-05</v>
+        <v>5.124833201183547E-05</v>
       </c>
       <c r="T15">
-        <v>0</v>
+        <v>8.702546945406021E-06</v>
       </c>
       <c r="U15">
-        <v>0.0007126543531619299</v>
+        <v>0.0007754936278017366</v>
       </c>
       <c r="V15">
-        <v>2.369196652798969E-05</v>
+        <v>4.157883540582877E-05</v>
       </c>
       <c r="W15">
-        <v>0.00105760938580946</v>
+        <v>0.001080082770890947</v>
       </c>
       <c r="X15">
-        <v>1.326750125567423E-05</v>
+        <v>1.837204355141271E-05</v>
       </c>
       <c r="Y15">
-        <v>4.169786108926186E-05</v>
+        <v>4.544663404823145E-05</v>
       </c>
       <c r="Z15">
-        <v>8.529107950076288E-06</v>
+        <v>1.063644626660736E-05</v>
       </c>
       <c r="AA15">
-        <v>6.538982761725154E-05</v>
+        <v>7.252122454505019E-05</v>
       </c>
       <c r="AB15">
-        <v>8.529107950076288E-06</v>
+        <v>8.702546945406021E-06</v>
       </c>
       <c r="AC15">
-        <v>9.476786611195875E-07</v>
+        <v>9.669496606006691E-07</v>
       </c>
       <c r="AD15">
         <v>0</v>
       </c>
       <c r="AE15">
-        <v>0.0003876005723979113</v>
+        <v>0.0003954824111856737</v>
       </c>
       <c r="AF15">
-        <v>0.00167833890884279</v>
+        <v>0.001712467848923785</v>
       </c>
       <c r="AG15">
         <v>0</v>
       </c>
       <c r="AH15">
-        <v>0.001039603491248188</v>
+        <v>0.001060743777678934</v>
       </c>
       <c r="AI15">
-        <v>0.001911467859478208</v>
+        <v>0.00195033746543155</v>
       </c>
     </row>
     <row r="16" spans="1:35">
@@ -2086,106 +2086,106 @@
         <v>14</v>
       </c>
       <c r="B16">
-        <v>0.007794656987708608</v>
+        <v>0.00747162002746137</v>
       </c>
       <c r="C16">
-        <v>0.001551349968252765</v>
+        <v>0.0015896652420275</v>
       </c>
       <c r="D16">
-        <v>0</v>
+        <v>2.610764083621807E-05</v>
       </c>
       <c r="E16">
-        <v>8.529107950076288E-06</v>
+        <v>4.447968438763078E-05</v>
       </c>
       <c r="F16">
-        <v>7.5814292889567E-06</v>
+        <v>5.124833201183547E-05</v>
       </c>
       <c r="G16">
-        <v>9.476786611195875E-07</v>
+        <v>1.643814423021138E-05</v>
       </c>
       <c r="H16">
-        <v>0.003621080164137944</v>
+        <v>0.003708251948403566</v>
       </c>
       <c r="I16">
         <v>0</v>
       </c>
       <c r="J16">
-        <v>9.476786611195875E-07</v>
+        <v>1.063644626660736E-05</v>
       </c>
       <c r="K16">
-        <v>9.476786611195875E-07</v>
+        <v>5.801697963604015E-06</v>
       </c>
       <c r="L16">
-        <v>0.002558732385022887</v>
+        <v>0.002682318358506256</v>
       </c>
       <c r="M16">
         <v>0</v>
       </c>
       <c r="N16">
-        <v>3.980250376702268E-05</v>
+        <v>6.865342590264751E-05</v>
       </c>
       <c r="O16">
-        <v>0.001444262279546251</v>
+        <v>0.001476532131737222</v>
       </c>
       <c r="P16">
-        <v>0.0001213028686233072</v>
+        <v>0.0001392407511264963</v>
       </c>
       <c r="Q16">
-        <v>0.001204499578282996</v>
+        <v>0.001255100659459669</v>
       </c>
       <c r="R16">
-        <v>0.003403114072080439</v>
+        <v>0.003492622174089617</v>
       </c>
       <c r="S16">
-        <v>2.179660920575052E-05</v>
+        <v>6.188477827844282E-05</v>
       </c>
       <c r="T16">
-        <v>0.000108035367367633</v>
+        <v>0.0001131331102902783</v>
       </c>
       <c r="U16">
-        <v>0.0002824082410136371</v>
+        <v>0.0003384323812102342</v>
       </c>
       <c r="V16">
-        <v>2.843035983358763E-06</v>
+        <v>3.287628846042275E-05</v>
       </c>
       <c r="W16">
-        <v>0.002678139896323955</v>
+        <v>0.002738401438821095</v>
       </c>
       <c r="X16">
-        <v>1.51628585779134E-05</v>
+        <v>2.030594287261405E-05</v>
       </c>
       <c r="Y16">
-        <v>9.476786611195875E-07</v>
+        <v>5.801697963604015E-06</v>
       </c>
       <c r="Z16">
-        <v>8.529107950076288E-06</v>
+        <v>1.160339592720803E-05</v>
       </c>
       <c r="AA16">
-        <v>0</v>
+        <v>1.547119456961071E-05</v>
       </c>
       <c r="AB16">
         <v>0</v>
       </c>
       <c r="AC16">
-        <v>1.231982259455464E-05</v>
+        <v>1.25703455878087E-05</v>
       </c>
       <c r="AD16">
         <v>0</v>
       </c>
       <c r="AE16">
-        <v>0.0005411245154992845</v>
+        <v>0.000552128256202982</v>
       </c>
       <c r="AF16">
-        <v>0.0002757744903858</v>
+        <v>0.0002813823512347947</v>
       </c>
       <c r="AG16">
-        <v>0</v>
+        <v>1.933899321201338E-06</v>
       </c>
       <c r="AH16">
         <v>0</v>
       </c>
       <c r="AI16">
-        <v>0.0005325954075492082</v>
+        <v>0.0005463265582393781</v>
       </c>
     </row>
     <row r="17" spans="1:35">
@@ -2193,106 +2193,106 @@
         <v>15</v>
       </c>
       <c r="B17">
-        <v>0.004189687360809696</v>
+        <v>0.003991568198959562</v>
       </c>
       <c r="C17">
-        <v>0.01045858170411577</v>
+        <v>0.01067512425303139</v>
       </c>
       <c r="D17">
-        <v>1.895357322239175E-06</v>
+        <v>2.320679185441606E-05</v>
       </c>
       <c r="E17">
-        <v>0</v>
+        <v>2.127289253321472E-05</v>
       </c>
       <c r="F17">
-        <v>7.960500753404536E-05</v>
+        <v>0.0001015297143630703</v>
       </c>
       <c r="G17">
-        <v>2.179660920575052E-05</v>
+        <v>3.190933879982208E-05</v>
       </c>
       <c r="H17">
-        <v>0.007231735863003573</v>
+        <v>0.007382660658686109</v>
       </c>
       <c r="I17">
         <v>0</v>
       </c>
       <c r="J17">
-        <v>0</v>
+        <v>1.933899321201338E-06</v>
       </c>
       <c r="K17">
-        <v>8.529107950076288E-06</v>
+        <v>1.740509389081204E-05</v>
       </c>
       <c r="L17">
-        <v>0.008076117550061126</v>
+        <v>0.00826451874915392</v>
       </c>
       <c r="M17">
         <v>0</v>
       </c>
       <c r="N17">
-        <v>0.0001317273338956227</v>
+        <v>0.0001479432980719024</v>
       </c>
       <c r="O17">
-        <v>0</v>
+        <v>1.933899321201338E-06</v>
       </c>
       <c r="P17">
-        <v>5.686071966717526E-06</v>
+        <v>1.547119456961071E-05</v>
       </c>
       <c r="Q17">
-        <v>0.001692554088759583</v>
+        <v>0.001737608540099402</v>
       </c>
       <c r="R17">
-        <v>0.005937206811914216</v>
+        <v>0.006081146415517608</v>
       </c>
       <c r="S17">
-        <v>1.895357322239175E-06</v>
+        <v>3.094238913922141E-05</v>
       </c>
       <c r="T17">
-        <v>1.895357322239175E-05</v>
+        <v>2.320679185441606E-05</v>
       </c>
       <c r="U17">
-        <v>0.0002255475213464618</v>
+        <v>0.0002639772573439827</v>
       </c>
       <c r="V17">
-        <v>1.326750125567423E-05</v>
+        <v>1.740509389081204E-05</v>
       </c>
       <c r="W17">
-        <v>0.001301162801717194</v>
+        <v>0.001346960877216732</v>
       </c>
       <c r="X17">
-        <v>2.843035983358763E-06</v>
+        <v>4.834748303003346E-06</v>
       </c>
       <c r="Y17">
-        <v>2.27442878668701E-05</v>
+        <v>2.51406911756174E-05</v>
       </c>
       <c r="Z17">
-        <v>0.0002426057372466144</v>
+        <v>0.0002504399620955733</v>
       </c>
       <c r="AA17">
-        <v>6.06514343116536E-05</v>
+        <v>6.671952658144617E-05</v>
       </c>
       <c r="AB17">
-        <v>2.843035983358763E-06</v>
+        <v>6.768647624204684E-06</v>
       </c>
       <c r="AC17">
-        <v>0.000151628585779134</v>
+        <v>0.0001547119456961071</v>
       </c>
       <c r="AD17">
         <v>0</v>
       </c>
       <c r="AE17">
-        <v>0.002302859146520598</v>
+        <v>0.002349687675259626</v>
       </c>
       <c r="AF17">
-        <v>0.000838695615090835</v>
+        <v>0.0008557504496315922</v>
       </c>
       <c r="AG17">
         <v>0</v>
       </c>
       <c r="AH17">
-        <v>0.0001696344803404062</v>
+        <v>0.0001750178885687211</v>
       </c>
       <c r="AI17">
-        <v>0.001345703698789814</v>
+        <v>0.001375002417374151</v>
       </c>
     </row>
     <row r="18" spans="1:35">
@@ -2300,88 +2300,88 @@
         <v>16</v>
       </c>
       <c r="B18">
-        <v>0.01579496024488017</v>
+        <v>0.01511245624552786</v>
       </c>
       <c r="C18">
-        <v>0.0002388150226021361</v>
+        <v>0.000254307760737976</v>
       </c>
       <c r="D18">
-        <v>0.002887576880431383</v>
+        <v>0.002988841400916668</v>
       </c>
       <c r="E18">
-        <v>0.006925635655461946</v>
+        <v>0.007170898683014563</v>
       </c>
       <c r="F18">
-        <v>0.004633200974213663</v>
+        <v>0.004792202517936916</v>
       </c>
       <c r="G18">
-        <v>0.008115920053828147</v>
+        <v>0.008331238275735365</v>
       </c>
       <c r="H18">
-        <v>0.003028781000938202</v>
+        <v>0.00310680925950995</v>
       </c>
       <c r="I18">
         <v>0</v>
       </c>
       <c r="J18">
-        <v>0.001486907819296633</v>
+        <v>0.001522945715446054</v>
       </c>
       <c r="K18">
-        <v>0.001234825295438823</v>
+        <v>0.001284109149277689</v>
       </c>
       <c r="L18">
-        <v>0.002442167909705177</v>
+        <v>0.002567251348894776</v>
       </c>
       <c r="M18">
-        <v>0.002900844381687057</v>
+        <v>0.002959832911098648</v>
       </c>
       <c r="N18">
-        <v>0.001889671250272458</v>
+        <v>0.00197934595524957</v>
       </c>
       <c r="O18">
-        <v>0.004286350584243895</v>
+        <v>0.004382215861842232</v>
       </c>
       <c r="P18">
-        <v>0.003707318922299827</v>
+        <v>0.003820418109033244</v>
       </c>
       <c r="Q18">
-        <v>0.005383762473820377</v>
+        <v>0.005546423253205438</v>
       </c>
       <c r="R18">
-        <v>7.107589958396906E-05</v>
+        <v>0.0001353729524840937</v>
       </c>
       <c r="S18">
-        <v>0.0006264155950000473</v>
+        <v>0.0007435842890019146</v>
       </c>
       <c r="T18">
-        <v>0.005487059447882412</v>
+        <v>0.005617977528089887</v>
       </c>
       <c r="U18">
-        <v>0.007531202319917362</v>
+        <v>0.007804250710708001</v>
       </c>
       <c r="V18">
-        <v>0.007718842694819041</v>
+        <v>0.007926086367943685</v>
       </c>
       <c r="W18">
-        <v>7.960500753404536E-05</v>
+        <v>0.0001044305633448723</v>
       </c>
       <c r="X18">
-        <v>0.0001743728736460041</v>
+        <v>0.0001817865361929258</v>
       </c>
       <c r="Y18">
-        <v>0.0002075416267851897</v>
+        <v>0.0002194975729563519</v>
       </c>
       <c r="Z18">
-        <v>6.728518493949071E-05</v>
+        <v>7.542207352685219E-05</v>
       </c>
       <c r="AA18">
-        <v>0.001029179025975872</v>
+        <v>0.001087818368175753</v>
       </c>
       <c r="AB18">
-        <v>0.001071824565726253</v>
+        <v>0.001096520915121159</v>
       </c>
       <c r="AC18">
-        <v>9.287250878971959E-05</v>
+        <v>9.476106673886557E-05</v>
       </c>
       <c r="AD18">
         <v>0</v>
@@ -2393,13 +2393,13 @@
         <v>0</v>
       </c>
       <c r="AG18">
-        <v>8.529107950076288E-06</v>
+        <v>1.740509389081204E-05</v>
       </c>
       <c r="AH18">
-        <v>0.001394035310506913</v>
+        <v>0.001423349900404185</v>
       </c>
       <c r="AI18">
-        <v>0.0004378275414372495</v>
+        <v>0.0004564002398035158</v>
       </c>
     </row>
     <row r="19" spans="1:35">
@@ -2407,13 +2407,13 @@
         <v>17</v>
       </c>
       <c r="B19">
-        <v>3.506411046142474E-05</v>
+        <v>3.287628846042275E-05</v>
       </c>
       <c r="C19">
-        <v>0.0008178466845462041</v>
+        <v>0.0008344775570983774</v>
       </c>
       <c r="D19">
-        <v>0</v>
+        <v>9.669496606006691E-07</v>
       </c>
       <c r="E19">
         <v>0</v>
@@ -2425,79 +2425,79 @@
         <v>0</v>
       </c>
       <c r="H19">
-        <v>0.001199761184977398</v>
+        <v>0.001224158270320447</v>
       </c>
       <c r="I19">
         <v>0</v>
       </c>
       <c r="J19">
-        <v>0</v>
+        <v>9.669496606006691E-07</v>
       </c>
       <c r="K19">
         <v>0</v>
       </c>
       <c r="L19">
-        <v>0.000632101666966765</v>
+        <v>0.0006449554236206463</v>
       </c>
       <c r="M19">
         <v>0</v>
       </c>
       <c r="N19">
-        <v>2.748268117246804E-05</v>
+        <v>2.80415401574194E-05</v>
       </c>
       <c r="O19">
-        <v>0.0006197818443722103</v>
+        <v>0.0006323850780328376</v>
       </c>
       <c r="P19">
         <v>0</v>
       </c>
       <c r="Q19">
-        <v>6.254679163389278E-05</v>
+        <v>6.381867759964416E-05</v>
       </c>
       <c r="R19">
-        <v>0.0105182854597663</v>
+        <v>0.01073314123266743</v>
       </c>
       <c r="S19">
-        <v>9.476786611195875E-06</v>
+        <v>9.669496606006692E-06</v>
       </c>
       <c r="T19">
-        <v>0.005472844267965619</v>
+        <v>0.005584134289968864</v>
       </c>
       <c r="U19">
-        <v>7.5814292889567E-06</v>
+        <v>7.735597284805353E-06</v>
       </c>
       <c r="V19">
-        <v>0.0002748268117246804</v>
+        <v>0.000280415401574194</v>
       </c>
       <c r="W19">
-        <v>0.0009865334862254906</v>
+        <v>0.001006594596685297</v>
       </c>
       <c r="X19">
-        <v>1.231982259455464E-05</v>
+        <v>1.25703455878087E-05</v>
       </c>
       <c r="Y19">
         <v>0</v>
       </c>
       <c r="Z19">
-        <v>5.686071966717526E-06</v>
+        <v>5.801697963604015E-06</v>
       </c>
       <c r="AA19">
-        <v>3.79071464447835E-06</v>
+        <v>3.867798642402676E-06</v>
       </c>
       <c r="AB19">
-        <v>5.686071966717525E-05</v>
+        <v>5.801697963604015E-05</v>
       </c>
       <c r="AC19">
-        <v>4.738393305597937E-06</v>
+        <v>4.834748303003346E-06</v>
       </c>
       <c r="AD19">
         <v>0</v>
       </c>
       <c r="AE19">
-        <v>7.486661422844741E-05</v>
+        <v>7.638902318745286E-05</v>
       </c>
       <c r="AF19">
-        <v>5.30700050226969E-05</v>
+        <v>5.414918099363747E-05</v>
       </c>
       <c r="AG19">
         <v>0</v>
@@ -2506,7 +2506,7 @@
         <v>0</v>
       </c>
       <c r="AI19">
-        <v>0.000383809857753433</v>
+        <v>0.000391614612543271</v>
       </c>
     </row>
     <row r="20" spans="1:35">
@@ -2514,106 +2514,106 @@
         <v>18</v>
       </c>
       <c r="B20">
-        <v>0.000595142199183101</v>
+        <v>0.0005879053936452068</v>
       </c>
       <c r="C20">
-        <v>0.007140758711536093</v>
+        <v>0.007286932642286643</v>
       </c>
       <c r="D20">
-        <v>6.918054226172989E-05</v>
+        <v>7.155427488444951E-05</v>
       </c>
       <c r="E20">
-        <v>0.0002132276987519072</v>
+        <v>0.0002175636736351506</v>
       </c>
       <c r="F20">
-        <v>6.444214895613195E-05</v>
+        <v>6.962037556324817E-05</v>
       </c>
       <c r="G20">
-        <v>0.0004340368267927711</v>
+        <v>0.0004438298942157071</v>
       </c>
       <c r="H20">
-        <v>0.005650060177594981</v>
+        <v>0.00576592082616179</v>
       </c>
       <c r="I20">
         <v>0</v>
       </c>
       <c r="J20">
-        <v>5.496536234493608E-05</v>
+        <v>5.705002997543948E-05</v>
       </c>
       <c r="K20">
-        <v>9.19248301286E-05</v>
+        <v>9.379411707826491E-05</v>
       </c>
       <c r="L20">
-        <v>0.003940447872935245</v>
+        <v>0.004022510588098783</v>
       </c>
       <c r="M20">
         <v>0</v>
       </c>
       <c r="N20">
-        <v>1.611053723903299E-05</v>
+        <v>1.740509389081204E-05</v>
       </c>
       <c r="O20">
-        <v>8.908179414524124E-05</v>
+        <v>9.08932680964629E-05</v>
       </c>
       <c r="P20">
-        <v>9.382018745083917E-05</v>
+        <v>9.572801639946625E-05</v>
       </c>
       <c r="Q20">
-        <v>0.000314629315491703</v>
+        <v>0.0003210272873194221</v>
       </c>
       <c r="R20">
-        <v>0.006393040247912738</v>
+        <v>0.006523042410412114</v>
       </c>
       <c r="S20">
-        <v>7.865732887292576E-05</v>
+        <v>8.12237714904562E-05</v>
       </c>
       <c r="T20">
-        <v>0.0001535239431013732</v>
+        <v>0.0001576127946779091</v>
       </c>
       <c r="U20">
-        <v>0.0003620132485476824</v>
+        <v>0.0003732425689918583</v>
       </c>
       <c r="V20">
-        <v>0.0008728120468911401</v>
+        <v>0.0008905606374132163</v>
       </c>
       <c r="W20">
-        <v>0.002142701452791388</v>
+        <v>0.002186273182618113</v>
       </c>
       <c r="X20">
-        <v>1.137214393343505E-05</v>
+        <v>1.160339592720803E-05</v>
       </c>
       <c r="Y20">
-        <v>0.0001108784033509917</v>
+        <v>0.000114100059950879</v>
       </c>
       <c r="Z20">
-        <v>1.705821590015258E-05</v>
+        <v>1.837204355141271E-05</v>
       </c>
       <c r="AA20">
-        <v>1.990125188351134E-05</v>
+        <v>2.030594287261405E-05</v>
       </c>
       <c r="AB20">
-        <v>0.0001857450175794392</v>
+        <v>0.0001895221334777311</v>
       </c>
       <c r="AC20">
-        <v>1.800589456127216E-05</v>
+        <v>1.837204355141271E-05</v>
       </c>
       <c r="AD20">
         <v>0</v>
       </c>
       <c r="AE20">
-        <v>0.00153903014565821</v>
+        <v>0.001570326248815487</v>
       </c>
       <c r="AF20">
-        <v>0.0004823684385098701</v>
+        <v>0.0004921773772457406</v>
       </c>
       <c r="AG20">
         <v>0</v>
       </c>
       <c r="AH20">
-        <v>0.0001980648401739938</v>
+        <v>0.0002020924790655399</v>
       </c>
       <c r="AI20">
-        <v>0.0007714104301513443</v>
+        <v>0.0007870970237289446</v>
       </c>
     </row>
     <row r="21" spans="1:35">
@@ -2621,106 +2621,106 @@
         <v>19</v>
       </c>
       <c r="B21">
-        <v>0.002698041148207466</v>
+        <v>0.002554681003306968</v>
       </c>
       <c r="C21">
-        <v>0.001942741255295155</v>
+        <v>0.001987081552534375</v>
       </c>
       <c r="D21">
-        <v>2.27442878668701E-05</v>
+        <v>2.610764083621807E-05</v>
       </c>
       <c r="E21">
-        <v>0.002828820803441969</v>
+        <v>0.002899882032141407</v>
       </c>
       <c r="F21">
-        <v>1.611053723903299E-05</v>
+        <v>2.610764083621807E-05</v>
       </c>
       <c r="G21">
-        <v>0.000762881322201268</v>
+        <v>0.0007880639733895454</v>
       </c>
       <c r="H21">
-        <v>0.005197069777579819</v>
+        <v>0.005313388385000677</v>
       </c>
       <c r="I21">
-        <v>4.454089707262062E-05</v>
+        <v>4.544663404823145E-05</v>
       </c>
       <c r="J21">
-        <v>2.748268117246804E-05</v>
+        <v>2.997543947862074E-05</v>
       </c>
       <c r="K21">
-        <v>5.686071966717526E-06</v>
+        <v>1.450424490901004E-05</v>
       </c>
       <c r="L21">
-        <v>0.001883037499644621</v>
+        <v>0.001931965421880137</v>
       </c>
       <c r="M21">
         <v>0</v>
       </c>
       <c r="N21">
-        <v>0.004287298262905014</v>
+        <v>0.004385116710824035</v>
       </c>
       <c r="O21">
-        <v>0.002972867959932146</v>
+        <v>0.003038155833607302</v>
       </c>
       <c r="P21">
-        <v>0.0004207693255370969</v>
+        <v>0.0004360942969309018</v>
       </c>
       <c r="Q21">
-        <v>0.0005420721941604041</v>
+        <v>0.0005811367460210021</v>
       </c>
       <c r="R21">
-        <v>0.00231991736242075</v>
+        <v>0.002374828366435244</v>
       </c>
       <c r="S21">
-        <v>0.00372342945953886</v>
+        <v>0.003816550310390841</v>
       </c>
       <c r="T21">
-        <v>0.0003278968167473773</v>
+        <v>0.0003345645825678315</v>
       </c>
       <c r="U21">
-        <v>0.0006226248803555691</v>
+        <v>0.000651724071244851</v>
       </c>
       <c r="V21">
-        <v>0.008529107950076288</v>
+        <v>0.008718985089636233</v>
       </c>
       <c r="W21">
-        <v>0.0006899100652950598</v>
+        <v>0.0007107080005414918</v>
       </c>
       <c r="X21">
-        <v>3.127339581694639E-05</v>
+        <v>3.77110367634261E-05</v>
       </c>
       <c r="Y21">
-        <v>0.0001051923313842742</v>
+        <v>0.0001082983619872749</v>
       </c>
       <c r="Z21">
-        <v>2.937803849470721E-05</v>
+        <v>2.997543947862074E-05</v>
       </c>
       <c r="AA21">
-        <v>0.0001838496602572</v>
+        <v>0.0001904890831383318</v>
       </c>
       <c r="AB21">
-        <v>3.695946778366391E-05</v>
+        <v>3.77110367634261E-05</v>
       </c>
       <c r="AC21">
         <v>0</v>
       </c>
       <c r="AD21">
-        <v>3.03257171558268E-05</v>
+        <v>3.094238913922141E-05</v>
       </c>
       <c r="AE21">
-        <v>0.002177765563252812</v>
+        <v>0.002222050320060338</v>
       </c>
       <c r="AF21">
-        <v>0.001725722841898769</v>
+        <v>0.001760815331953818</v>
       </c>
       <c r="AG21">
-        <v>0</v>
+        <v>9.669496606006691E-07</v>
       </c>
       <c r="AH21">
-        <v>0.0001412041205068186</v>
+        <v>0.0001440754994294997</v>
       </c>
       <c r="AI21">
-        <v>0.002863884913903394</v>
+        <v>0.002922121874335222</v>
       </c>
     </row>
     <row r="22" spans="1:35">
@@ -2728,106 +2728,106 @@
         <v>20</v>
       </c>
       <c r="B22">
-        <v>0.007208991575136703</v>
+        <v>0.0069368968651492</v>
       </c>
       <c r="C22">
-        <v>0.004141355749092598</v>
+        <v>0.004235239513430931</v>
       </c>
       <c r="D22">
-        <v>1.042446527231546E-05</v>
+        <v>3.384323812102342E-05</v>
       </c>
       <c r="E22">
-        <v>0.003931918764985168</v>
+        <v>0.004042816530971397</v>
       </c>
       <c r="F22">
-        <v>1.326750125567423E-05</v>
+        <v>5.221528167243614E-05</v>
       </c>
       <c r="G22">
-        <v>0.0002141753774130268</v>
+        <v>0.0002407704654895666</v>
       </c>
       <c r="H22">
-        <v>0.004418077918139517</v>
+        <v>0.00452339051228993</v>
       </c>
       <c r="I22">
         <v>0</v>
       </c>
       <c r="J22">
-        <v>9.476786611195875E-07</v>
+        <v>6.768647624204684E-06</v>
       </c>
       <c r="K22">
-        <v>0</v>
+        <v>3.867798642402676E-06</v>
       </c>
       <c r="L22">
-        <v>0.002801338122269501</v>
+        <v>0.002877642189947591</v>
       </c>
       <c r="M22">
         <v>0</v>
       </c>
       <c r="N22">
-        <v>0.0002748268117246804</v>
+        <v>0.0002949196464832041</v>
       </c>
       <c r="O22">
-        <v>4.359321841150103E-05</v>
+        <v>4.834748303003345E-05</v>
       </c>
       <c r="P22">
-        <v>2.179660920575052E-05</v>
+        <v>4.157883540582877E-05</v>
       </c>
       <c r="Q22">
-        <v>0.0003857052150756721</v>
+        <v>0.0004254578506642944</v>
       </c>
       <c r="R22">
-        <v>0.009042749784403104</v>
+        <v>0.009255642151269604</v>
       </c>
       <c r="S22">
-        <v>0.0002189137707186247</v>
+        <v>0.0002620433580227813</v>
       </c>
       <c r="T22">
-        <v>0.001849868746505435</v>
+        <v>0.001898122183759114</v>
       </c>
       <c r="U22">
-        <v>0.0009618938410363814</v>
+        <v>0.001026900539557911</v>
       </c>
       <c r="V22">
-        <v>0.0001563669790847319</v>
+        <v>0.0001846873851747278</v>
       </c>
       <c r="W22">
-        <v>0.0008775504401967381</v>
+        <v>0.0008992631843586223</v>
       </c>
       <c r="X22">
-        <v>0</v>
+        <v>9.669496606006691E-07</v>
       </c>
       <c r="Y22">
-        <v>1.137214393343505E-05</v>
+        <v>1.450424490901004E-05</v>
       </c>
       <c r="Z22">
-        <v>0.0004501473640318041</v>
+        <v>0.0004602680384459185</v>
       </c>
       <c r="AA22">
-        <v>4.169786108926186E-05</v>
+        <v>5.511613065423814E-05</v>
       </c>
       <c r="AB22">
-        <v>4.738393305597937E-06</v>
+        <v>5.801697963604015E-06</v>
       </c>
       <c r="AC22">
-        <v>6.633750627837113E-06</v>
+        <v>6.768647624204684E-06</v>
       </c>
       <c r="AD22">
         <v>0</v>
       </c>
       <c r="AE22">
-        <v>0.002028032334795917</v>
+        <v>0.002069272273685432</v>
       </c>
       <c r="AF22">
-        <v>0.004536537750779466</v>
+        <v>0.004628788025295403</v>
       </c>
       <c r="AG22">
-        <v>0</v>
+        <v>3.867798642402676E-06</v>
       </c>
       <c r="AH22">
-        <v>5.686071966717526E-06</v>
+        <v>5.801697963604015E-06</v>
       </c>
       <c r="AI22">
-        <v>0.0006434738109001999</v>
+        <v>0.0006613935678508577</v>
       </c>
     </row>
     <row r="23" spans="1:35">
@@ -2835,88 +2835,88 @@
         <v>21</v>
       </c>
       <c r="B23">
-        <v>0.008096018801944637</v>
+        <v>0.007754936278017367</v>
       </c>
       <c r="C23">
-        <v>2.179660920575052E-05</v>
+        <v>3.287628846042275E-05</v>
       </c>
       <c r="D23">
-        <v>0.0005904038058775031</v>
+        <v>0.0006198147324450289</v>
       </c>
       <c r="E23">
-        <v>0.0004122402175870206</v>
+        <v>0.0004602680384459185</v>
       </c>
       <c r="F23">
-        <v>0.0006254679163389278</v>
+        <v>0.000672030014117465</v>
       </c>
       <c r="G23">
-        <v>0.002352138436898816</v>
+        <v>0.002420275000483475</v>
       </c>
       <c r="H23">
-        <v>5.117464770045773E-05</v>
+        <v>6.671952658144617E-05</v>
       </c>
       <c r="I23">
         <v>0</v>
       </c>
       <c r="J23">
-        <v>0.0007590906075567896</v>
+        <v>0.000783229225086542</v>
       </c>
       <c r="K23">
-        <v>0.0001336226912178619</v>
+        <v>0.0001440754994294997</v>
       </c>
       <c r="L23">
-        <v>0.0001847973389183196</v>
+        <v>0.0002388365661683653</v>
       </c>
       <c r="M23">
-        <v>6.06514343116536E-05</v>
+        <v>6.188477827844282E-05</v>
       </c>
       <c r="N23">
-        <v>0.0008898702627912927</v>
+        <v>0.0009311725231584444</v>
       </c>
       <c r="O23">
-        <v>0.0005619734460439155</v>
+        <v>0.0005772689473785994</v>
       </c>
       <c r="P23">
-        <v>0.0006434738109001999</v>
+        <v>0.0006816995107234718</v>
       </c>
       <c r="Q23">
-        <v>5.591304100605567E-05</v>
+        <v>9.669496606006691E-05</v>
       </c>
       <c r="R23">
-        <v>9.476786611195875E-07</v>
+        <v>2.030594287261405E-05</v>
       </c>
       <c r="S23">
-        <v>0.0006264155950000473</v>
+        <v>0.0006778317120810691</v>
       </c>
       <c r="T23">
-        <v>0.0002501871665355711</v>
+        <v>0.000265911156665184</v>
       </c>
       <c r="U23">
-        <v>0.001635693369092408</v>
+        <v>0.001736641590438802</v>
       </c>
       <c r="V23">
-        <v>0.000887027226807934</v>
+        <v>0.0009379411707826491</v>
       </c>
       <c r="W23">
-        <v>0</v>
+        <v>8.702546945406021E-06</v>
       </c>
       <c r="X23">
-        <v>3.222107447806598E-05</v>
+        <v>4.351273472703011E-05</v>
       </c>
       <c r="Y23">
-        <v>0.0002975710995915505</v>
+        <v>0.0003074899920710128</v>
       </c>
       <c r="Z23">
-        <v>1.990125188351134E-05</v>
+        <v>2.320679185441606E-05</v>
       </c>
       <c r="AA23">
-        <v>0.0002767221690469196</v>
+        <v>0.0002939526968226034</v>
       </c>
       <c r="AB23">
-        <v>0.0005477582661271216</v>
+        <v>0.0005608308031483881</v>
       </c>
       <c r="AC23">
-        <v>0.0001364657272012206</v>
+        <v>0.0001392407511264963</v>
       </c>
       <c r="AD23">
         <v>0</v>
@@ -2928,13 +2928,13 @@
         <v>0</v>
       </c>
       <c r="AG23">
-        <v>5.686071966717526E-06</v>
+        <v>5.801697963604015E-06</v>
       </c>
       <c r="AH23">
-        <v>0.0006520029188502763</v>
+        <v>0.0006652613664932603</v>
       </c>
       <c r="AI23">
-        <v>1.51628585779134E-05</v>
+        <v>1.740509389081204E-05</v>
       </c>
     </row>
     <row r="24" spans="1:35">
@@ -2942,25 +2942,25 @@
         <v>22</v>
       </c>
       <c r="B24">
-        <v>0.0002046985908018309</v>
+        <v>0.0002020924790655399</v>
       </c>
       <c r="C24">
-        <v>0.0008150036485628453</v>
+        <v>0.0008315767081165755</v>
       </c>
       <c r="D24">
-        <v>1.895357322239175E-06</v>
+        <v>1.933899321201338E-06</v>
       </c>
       <c r="E24">
-        <v>5.686071966717526E-06</v>
+        <v>5.801697963604015E-06</v>
       </c>
       <c r="F24">
-        <v>4.738393305597937E-06</v>
+        <v>5.801697963604015E-06</v>
       </c>
       <c r="G24">
-        <v>5.686071966717526E-06</v>
+        <v>5.801697963604015E-06</v>
       </c>
       <c r="H24">
-        <v>0.000232181271974299</v>
+        <v>0.0002369026668471639</v>
       </c>
       <c r="I24">
         <v>0</v>
@@ -2972,55 +2972,55 @@
         <v>0</v>
       </c>
       <c r="L24">
-        <v>0.0003639086058699216</v>
+        <v>0.0003722756193312576</v>
       </c>
       <c r="M24">
         <v>0</v>
       </c>
       <c r="N24">
-        <v>4.738393305597937E-06</v>
+        <v>4.834748303003346E-06</v>
       </c>
       <c r="O24">
-        <v>3.695946778366391E-05</v>
+        <v>3.77110367634261E-05</v>
       </c>
       <c r="P24">
-        <v>9.476786611195875E-06</v>
+        <v>9.669496606006692E-06</v>
       </c>
       <c r="Q24">
-        <v>9.476786611195875E-06</v>
+        <v>1.063644626660736E-05</v>
       </c>
       <c r="R24">
-        <v>0.0001876403749016783</v>
+        <v>0.0001914560327989325</v>
       </c>
       <c r="S24">
-        <v>2.843035983358763E-06</v>
+        <v>3.867798642402676E-06</v>
       </c>
       <c r="T24">
-        <v>0.000124145904606666</v>
+        <v>0.0001266704055386877</v>
       </c>
       <c r="U24">
-        <v>4.833161171709897E-05</v>
+        <v>5.02813823512348E-05</v>
       </c>
       <c r="V24">
-        <v>9.476786611195875E-06</v>
+        <v>9.669496606006692E-06</v>
       </c>
       <c r="W24">
-        <v>9.19248301286E-05</v>
+        <v>9.379411707826491E-05</v>
       </c>
       <c r="X24">
-        <v>7.5814292889567E-05</v>
+        <v>7.83229225086542E-05</v>
       </c>
       <c r="Y24">
-        <v>7.5814292889567E-06</v>
+        <v>7.735597284805353E-06</v>
       </c>
       <c r="Z24">
-        <v>9.476786611195875E-07</v>
+        <v>9.669496606006691E-07</v>
       </c>
       <c r="AA24">
-        <v>0</v>
+        <v>9.669496606006691E-07</v>
       </c>
       <c r="AB24">
-        <v>3.79071464447835E-06</v>
+        <v>3.867798642402676E-06</v>
       </c>
       <c r="AC24">
         <v>0</v>
@@ -3029,10 +3029,10 @@
         <v>0</v>
       </c>
       <c r="AE24">
-        <v>5.212232636157732E-05</v>
+        <v>5.31822313330368E-05</v>
       </c>
       <c r="AF24">
-        <v>1.421517991679381E-05</v>
+        <v>1.450424490901004E-05</v>
       </c>
       <c r="AG24">
         <v>0</v>
@@ -3041,7 +3041,7 @@
         <v>0</v>
       </c>
       <c r="AI24">
-        <v>1.800589456127216E-05</v>
+        <v>1.837204355141271E-05</v>
       </c>
     </row>
     <row r="25" spans="1:35">
@@ -3049,85 +3049,85 @@
         <v>23</v>
       </c>
       <c r="B25">
-        <v>0.005553396954160783</v>
+        <v>0.005295983291109865</v>
       </c>
       <c r="C25">
-        <v>0.000519327906293534</v>
+        <v>0.0005327892629909687</v>
       </c>
       <c r="D25">
-        <v>3.79071464447835E-06</v>
+        <v>1.063644626660736E-05</v>
       </c>
       <c r="E25">
-        <v>5.875607698941443E-05</v>
+        <v>9.282716741766424E-05</v>
       </c>
       <c r="F25">
-        <v>0</v>
+        <v>4.254578506642944E-05</v>
       </c>
       <c r="G25">
-        <v>9.476786611195875E-07</v>
+        <v>1.547119456961071E-05</v>
       </c>
       <c r="H25">
-        <v>0.0002748268117246804</v>
+        <v>0.0002842832002165967</v>
       </c>
       <c r="I25">
         <v>0</v>
       </c>
       <c r="J25">
-        <v>0</v>
+        <v>5.801697963604015E-06</v>
       </c>
       <c r="K25">
-        <v>2.843035983358763E-06</v>
+        <v>1.063644626660736E-05</v>
       </c>
       <c r="L25">
-        <v>0.0003051525288805072</v>
+        <v>0.0003510027267980429</v>
       </c>
       <c r="M25">
         <v>0</v>
       </c>
       <c r="N25">
-        <v>9.476786611195875E-07</v>
+        <v>2.223984219381539E-05</v>
       </c>
       <c r="O25">
-        <v>0.0003079955648638659</v>
+        <v>0.0003200603376588215</v>
       </c>
       <c r="P25">
-        <v>1.231982259455464E-05</v>
+        <v>2.707459049681873E-05</v>
       </c>
       <c r="Q25">
-        <v>3.222107447806598E-05</v>
+        <v>6.285172793904349E-05</v>
       </c>
       <c r="R25">
-        <v>0.001150481894599179</v>
+        <v>0.001191281981860024</v>
       </c>
       <c r="S25">
-        <v>6.633750627837113E-06</v>
+        <v>4.351273472703011E-05</v>
       </c>
       <c r="T25">
-        <v>0.0002151230560741464</v>
+        <v>0.0002282001199017579</v>
       </c>
       <c r="U25">
-        <v>5.212232636157732E-05</v>
+        <v>8.605851979345956E-05</v>
       </c>
       <c r="V25">
-        <v>1.895357322239175E-06</v>
+        <v>1.740509389081204E-05</v>
       </c>
       <c r="W25">
-        <v>0.0001933264468683959</v>
+        <v>0.0002049933280473419</v>
       </c>
       <c r="X25">
-        <v>0</v>
+        <v>1.933899321201338E-06</v>
       </c>
       <c r="Y25">
-        <v>0</v>
+        <v>2.900848981802008E-06</v>
       </c>
       <c r="Z25">
-        <v>2.843035983358763E-06</v>
+        <v>7.735597284805353E-06</v>
       </c>
       <c r="AA25">
-        <v>0</v>
+        <v>6.768647624204684E-06</v>
       </c>
       <c r="AB25">
-        <v>9.476786611195875E-07</v>
+        <v>3.867798642402676E-06</v>
       </c>
       <c r="AC25">
         <v>0</v>
@@ -3142,13 +3142,13 @@
         <v>0</v>
       </c>
       <c r="AG25">
-        <v>0</v>
+        <v>9.669496606006691E-07</v>
       </c>
       <c r="AH25">
-        <v>9.476786611195875E-07</v>
+        <v>9.669496606006691E-07</v>
       </c>
       <c r="AI25">
-        <v>0</v>
+        <v>2.900848981802008E-06</v>
       </c>
     </row>
     <row r="26" spans="1:35">
@@ -3156,25 +3156,25 @@
         <v>24</v>
       </c>
       <c r="B26">
-        <v>0.0004349845054538907</v>
+        <v>0.0004225570016824924</v>
       </c>
       <c r="C26">
-        <v>0.002064991802579581</v>
+        <v>0.002106983310448858</v>
       </c>
       <c r="D26">
-        <v>9.476786611195875E-07</v>
+        <v>9.669496606006691E-07</v>
       </c>
       <c r="E26">
-        <v>4.738393305597938E-05</v>
+        <v>5.124833201183547E-05</v>
       </c>
       <c r="F26">
-        <v>4.738393305597937E-06</v>
+        <v>5.801697963604015E-06</v>
       </c>
       <c r="G26">
         <v>0</v>
       </c>
       <c r="H26">
-        <v>0.000703177566550734</v>
+        <v>0.0007184435978262972</v>
       </c>
       <c r="I26">
         <v>0</v>
@@ -3186,49 +3186,49 @@
         <v>0</v>
       </c>
       <c r="L26">
-        <v>2.463964518910928E-05</v>
+        <v>2.80415401574194E-05</v>
       </c>
       <c r="M26">
         <v>0</v>
       </c>
       <c r="N26">
-        <v>9.476786611195875E-07</v>
+        <v>1.933899321201338E-06</v>
       </c>
       <c r="O26">
         <v>0</v>
       </c>
       <c r="P26">
-        <v>2.843035983358763E-06</v>
+        <v>3.867798642402676E-06</v>
       </c>
       <c r="Q26">
         <v>0</v>
       </c>
       <c r="R26">
-        <v>0.0001393087631845794</v>
+        <v>0.0001440754994294997</v>
       </c>
       <c r="S26">
-        <v>4.738393305597937E-06</v>
+        <v>9.669496606006692E-06</v>
       </c>
       <c r="T26">
-        <v>8.529107950076288E-06</v>
+        <v>8.702546945406021E-06</v>
       </c>
       <c r="U26">
-        <v>0</v>
+        <v>3.867798642402676E-06</v>
       </c>
       <c r="V26">
-        <v>0</v>
+        <v>9.669496606006691E-07</v>
       </c>
       <c r="W26">
-        <v>0.000264402346452365</v>
+        <v>0.0002697789553075867</v>
       </c>
       <c r="X26">
-        <v>3.79071464447835E-06</v>
+        <v>3.867798642402676E-06</v>
       </c>
       <c r="Y26">
         <v>0</v>
       </c>
       <c r="Z26">
-        <v>9.476786611195875E-07</v>
+        <v>9.669496606006691E-07</v>
       </c>
       <c r="AA26">
         <v>0</v>
@@ -3243,7 +3243,7 @@
         <v>0</v>
       </c>
       <c r="AE26">
-        <v>0.0001914310895461567</v>
+        <v>0.0001953238314413352</v>
       </c>
       <c r="AF26">
         <v>0</v>
@@ -3263,10 +3263,10 @@
         <v>25</v>
       </c>
       <c r="B27">
-        <v>0.0001582623364069711</v>
+        <v>0.000143108549768899</v>
       </c>
       <c r="C27">
-        <v>0.0008633352602799443</v>
+        <v>0.0008808911408072096</v>
       </c>
       <c r="D27">
         <v>0</v>
@@ -3275,13 +3275,13 @@
         <v>0</v>
       </c>
       <c r="F27">
-        <v>0</v>
+        <v>9.669496606006691E-07</v>
       </c>
       <c r="G27">
         <v>0</v>
       </c>
       <c r="H27">
-        <v>0.001987282152367775</v>
+        <v>0.002028660387940204</v>
       </c>
       <c r="I27">
         <v>0</v>
@@ -3293,40 +3293,40 @@
         <v>0</v>
       </c>
       <c r="L27">
-        <v>0.001225348508827627</v>
+        <v>0.001253166760138467</v>
       </c>
       <c r="M27">
         <v>0</v>
       </c>
       <c r="N27">
-        <v>7.676197155068659E-05</v>
+        <v>7.928987216925487E-05</v>
       </c>
       <c r="O27">
-        <v>1.042446527231546E-05</v>
+        <v>1.160339592720803E-05</v>
       </c>
       <c r="P27">
-        <v>1.611053723903299E-05</v>
+        <v>1.643814423021138E-05</v>
       </c>
       <c r="Q27">
-        <v>0.000259663953146767</v>
+        <v>0.0002649442070045833</v>
       </c>
       <c r="R27">
-        <v>6.444214895613195E-05</v>
+        <v>6.57525769208455E-05</v>
       </c>
       <c r="S27">
-        <v>0</v>
+        <v>3.867798642402676E-06</v>
       </c>
       <c r="T27">
-        <v>0.0001137214393343505</v>
+        <v>0.0001160339592720803</v>
       </c>
       <c r="U27">
-        <v>0</v>
+        <v>1.933899321201338E-06</v>
       </c>
       <c r="V27">
-        <v>0.00218345163521953</v>
+        <v>0.002228818967684542</v>
       </c>
       <c r="W27">
-        <v>0.0001772159096293629</v>
+        <v>0.0001808195865323251</v>
       </c>
       <c r="X27">
         <v>0</v>
@@ -3335,13 +3335,13 @@
         <v>0</v>
       </c>
       <c r="Z27">
-        <v>9.476786611195875E-07</v>
+        <v>9.669496606006691E-07</v>
       </c>
       <c r="AA27">
-        <v>0</v>
+        <v>2.900848981802008E-06</v>
       </c>
       <c r="AB27">
-        <v>4.359321841150103E-05</v>
+        <v>4.641358370883212E-05</v>
       </c>
       <c r="AC27">
         <v>0</v>
@@ -3353,7 +3353,7 @@
         <v>0</v>
       </c>
       <c r="AF27">
-        <v>0.0002511348451966907</v>
+        <v>0.0002562416600591773</v>
       </c>
       <c r="AG27">
         <v>0</v>
@@ -3370,25 +3370,25 @@
         <v>26</v>
       </c>
       <c r="B28">
-        <v>0.0001980648401739938</v>
+        <v>0.0001885551838171305</v>
       </c>
       <c r="C28">
-        <v>0.0008036315046294103</v>
+        <v>0.0008199733121893674</v>
       </c>
       <c r="D28">
-        <v>4.738393305597937E-06</v>
+        <v>4.834748303003346E-06</v>
       </c>
       <c r="E28">
-        <v>1.137214393343505E-05</v>
+        <v>1.160339592720803E-05</v>
       </c>
       <c r="F28">
-        <v>0</v>
+        <v>5.801697963604015E-06</v>
       </c>
       <c r="G28">
-        <v>0</v>
+        <v>1.933899321201338E-06</v>
       </c>
       <c r="H28">
-        <v>0.002064991802579581</v>
+        <v>0.002106983310448858</v>
       </c>
       <c r="I28">
         <v>0</v>
@@ -3400,28 +3400,28 @@
         <v>0</v>
       </c>
       <c r="L28">
-        <v>0.001552297646913884</v>
+        <v>0.001583863544063896</v>
       </c>
       <c r="M28">
         <v>0</v>
       </c>
       <c r="N28">
-        <v>7.5814292889567E-05</v>
+        <v>7.928987216925487E-05</v>
       </c>
       <c r="O28">
-        <v>0.0007069682811952123</v>
+        <v>0.0007213444468080992</v>
       </c>
       <c r="P28">
-        <v>3.79071464447835E-06</v>
+        <v>3.867798642402676E-06</v>
       </c>
       <c r="Q28">
-        <v>8.529107950076289E-05</v>
+        <v>8.702546945406022E-05</v>
       </c>
       <c r="R28">
-        <v>0.0001089830460287526</v>
+        <v>0.000111199210969077</v>
       </c>
       <c r="S28">
-        <v>9.476786611195875E-07</v>
+        <v>3.867798642402676E-06</v>
       </c>
       <c r="T28">
         <v>0</v>
@@ -3430,10 +3430,10 @@
         <v>0</v>
       </c>
       <c r="V28">
-        <v>6.633750627837113E-06</v>
+        <v>7.735597284805353E-06</v>
       </c>
       <c r="W28">
-        <v>0.0001573146577458515</v>
+        <v>0.0001605136436597111</v>
       </c>
       <c r="X28">
         <v>0</v>
@@ -3442,7 +3442,7 @@
         <v>0</v>
       </c>
       <c r="Z28">
-        <v>1.895357322239175E-05</v>
+        <v>1.933899321201338E-05</v>
       </c>
       <c r="AA28">
         <v>0</v>
@@ -3460,7 +3460,7 @@
         <v>0</v>
       </c>
       <c r="AF28">
-        <v>0.0007780441807791814</v>
+        <v>0.0007938656713531493</v>
       </c>
       <c r="AG28">
         <v>0</v>
@@ -3477,16 +3477,16 @@
         <v>27</v>
       </c>
       <c r="B29">
-        <v>6.633750627837113E-06</v>
+        <v>6.768647624204684E-06</v>
       </c>
       <c r="C29">
-        <v>0.0002861989556581155</v>
+        <v>0.0002920187975014021</v>
       </c>
       <c r="D29">
         <v>0</v>
       </c>
       <c r="E29">
-        <v>1.705821590015258E-05</v>
+        <v>1.740509389081204E-05</v>
       </c>
       <c r="F29">
         <v>0</v>
@@ -3495,7 +3495,7 @@
         <v>0</v>
       </c>
       <c r="H29">
-        <v>0.001246197439372258</v>
+        <v>0.00127153880368988</v>
       </c>
       <c r="I29">
         <v>0</v>
@@ -3507,7 +3507,7 @@
         <v>0</v>
       </c>
       <c r="L29">
-        <v>0.0005970375565053402</v>
+        <v>0.0006091782861784216</v>
       </c>
       <c r="M29">
         <v>0</v>
@@ -3522,10 +3522,10 @@
         <v>0</v>
       </c>
       <c r="Q29">
-        <v>2.179660920575052E-05</v>
+        <v>2.223984219381539E-05</v>
       </c>
       <c r="R29">
-        <v>9.476786611195875E-07</v>
+        <v>9.669496606006691E-07</v>
       </c>
       <c r="S29">
         <v>0</v>
@@ -3540,7 +3540,7 @@
         <v>0</v>
       </c>
       <c r="W29">
-        <v>8.813411548412165E-05</v>
+        <v>8.992631843586223E-05</v>
       </c>
       <c r="X29">
         <v>0</v>
@@ -3567,7 +3567,7 @@
         <v>0</v>
       </c>
       <c r="AF29">
-        <v>1.705821590015258E-05</v>
+        <v>1.740509389081204E-05</v>
       </c>
       <c r="AG29">
         <v>0</v>
@@ -3602,7 +3602,7 @@
         <v>0</v>
       </c>
       <c r="H30">
-        <v>3.411643180030515E-05</v>
+        <v>3.481018778162409E-05</v>
       </c>
       <c r="I30">
         <v>0</v>
@@ -3683,7 +3683,7 @@
         <v>0</v>
       </c>
       <c r="AI30">
-        <v>8.150036485628454E-05</v>
+        <v>8.315767081165754E-05</v>
       </c>
     </row>
     <row r="31" spans="1:35">
@@ -3691,88 +3691,88 @@
         <v>29</v>
       </c>
       <c r="B31">
-        <v>0.005668066072156253</v>
+        <v>0.00541878589800615</v>
       </c>
       <c r="C31">
-        <v>0</v>
+        <v>5.801697963604015E-06</v>
       </c>
       <c r="D31">
-        <v>3.601178912254433E-05</v>
+        <v>5.898392929664082E-05</v>
       </c>
       <c r="E31">
-        <v>0.0005344907648714474</v>
+        <v>0.0005850045446634048</v>
       </c>
       <c r="F31">
-        <v>1.800589456127216E-05</v>
+        <v>3.094238913922141E-05</v>
       </c>
       <c r="G31">
-        <v>3.222107447806598E-05</v>
+        <v>4.254578506642944E-05</v>
       </c>
       <c r="H31">
-        <v>0.0007884686460514969</v>
+        <v>0.0008190063625287667</v>
       </c>
       <c r="I31">
         <v>0</v>
       </c>
       <c r="J31">
-        <v>9.476786611195875E-06</v>
+        <v>1.25703455878087E-05</v>
       </c>
       <c r="K31">
-        <v>1.137214393343505E-05</v>
+        <v>1.353729524840937E-05</v>
       </c>
       <c r="L31">
-        <v>7.5814292889567E-06</v>
+        <v>5.124833201183547E-05</v>
       </c>
       <c r="M31">
-        <v>0.001046237241876025</v>
+        <v>0.001067512425303139</v>
       </c>
       <c r="N31">
-        <v>0.0001487855497957753</v>
+        <v>0.0001643814423021138</v>
       </c>
       <c r="O31">
-        <v>0.001298319765733835</v>
+        <v>0.001325687984683517</v>
       </c>
       <c r="P31">
-        <v>0.0006482122042057979</v>
+        <v>0.0006739639134386664</v>
       </c>
       <c r="Q31">
-        <v>0.002464912197572047</v>
+        <v>0.002540176758397958</v>
       </c>
       <c r="R31">
-        <v>0</v>
+        <v>1.933899321201338E-05</v>
       </c>
       <c r="S31">
-        <v>4.359321841150103E-05</v>
+        <v>9.862886538126825E-05</v>
       </c>
       <c r="T31">
-        <v>0.0001810066242738412</v>
+        <v>0.0001885551838171305</v>
       </c>
       <c r="U31">
-        <v>0.0003885482510590309</v>
+        <v>0.0004457637935369084</v>
       </c>
       <c r="V31">
-        <v>0.0002871466343192351</v>
+        <v>0.0003036221934286101</v>
       </c>
       <c r="W31">
-        <v>1.895357322239175E-06</v>
+        <v>1.450424490901004E-05</v>
       </c>
       <c r="X31">
-        <v>0</v>
+        <v>9.669496606006691E-07</v>
       </c>
       <c r="Y31">
-        <v>0.001153324930582538</v>
+        <v>0.001180645535593417</v>
       </c>
       <c r="Z31">
-        <v>1.895357322239175E-06</v>
+        <v>1.933899321201338E-06</v>
       </c>
       <c r="AA31">
-        <v>6.349447029501236E-05</v>
+        <v>6.671952658144617E-05</v>
       </c>
       <c r="AB31">
-        <v>0.0005610257673827958</v>
+        <v>0.0005743680983967975</v>
       </c>
       <c r="AC31">
-        <v>2.179660920575052E-05</v>
+        <v>2.223984219381539E-05</v>
       </c>
       <c r="AD31">
         <v>0</v>
@@ -3790,7 +3790,7 @@
         <v>0</v>
       </c>
       <c r="AI31">
-        <v>0</v>
+        <v>1.933899321201338E-06</v>
       </c>
     </row>
     <row r="32" spans="1:35">
@@ -3798,88 +3798,88 @@
         <v>30</v>
       </c>
       <c r="B32">
-        <v>0.00965021180618076</v>
+        <v>0.009249840453306001</v>
       </c>
       <c r="C32">
-        <v>9.476786611195875E-07</v>
+        <v>5.801697963604015E-06</v>
       </c>
       <c r="D32">
-        <v>3.79071464447835E-06</v>
+        <v>2.997543947862074E-05</v>
       </c>
       <c r="E32">
-        <v>1.51628585779134E-05</v>
+        <v>6.962037556324817E-05</v>
       </c>
       <c r="F32">
-        <v>1.231982259455464E-05</v>
+        <v>4.931443269063413E-05</v>
       </c>
       <c r="G32">
-        <v>0.0001364657272012206</v>
+        <v>0.0001769517878899224</v>
       </c>
       <c r="H32">
-        <v>0.0002748268117246804</v>
+        <v>0.0003007213444468081</v>
       </c>
       <c r="I32">
         <v>0</v>
       </c>
       <c r="J32">
-        <v>0</v>
+        <v>1.353729524840937E-05</v>
       </c>
       <c r="K32">
-        <v>2.558732385022886E-05</v>
+        <v>3.674408710282543E-05</v>
       </c>
       <c r="L32">
-        <v>3.316875313918556E-05</v>
+        <v>7.058732522384885E-05</v>
       </c>
       <c r="M32">
         <v>0</v>
       </c>
       <c r="N32">
-        <v>0.0002141753774130268</v>
+        <v>0.0002378696165077646</v>
       </c>
       <c r="O32">
-        <v>9.476786611195875E-07</v>
+        <v>1.450424490901004E-05</v>
       </c>
       <c r="P32">
-        <v>0.0004444612920650866</v>
+        <v>0.0004844417799609353</v>
       </c>
       <c r="Q32">
-        <v>0.0005212232636157731</v>
+        <v>0.0005695333500937941</v>
       </c>
       <c r="R32">
-        <v>0</v>
+        <v>4.738053336943278E-05</v>
       </c>
       <c r="S32">
-        <v>1.895357322239175E-06</v>
+        <v>6.768647624204685E-05</v>
       </c>
       <c r="T32">
-        <v>0</v>
+        <v>8.702546945406021E-06</v>
       </c>
       <c r="U32">
-        <v>0.0004681532585930763</v>
+        <v>0.0005463265582393781</v>
       </c>
       <c r="V32">
-        <v>0.0002738791330635608</v>
+        <v>0.0003103908410528148</v>
       </c>
       <c r="W32">
-        <v>0</v>
+        <v>3.867798642402676E-06</v>
       </c>
       <c r="X32">
-        <v>0</v>
+        <v>4.834748303003346E-06</v>
       </c>
       <c r="Y32">
-        <v>0</v>
+        <v>5.801697963604015E-06</v>
       </c>
       <c r="Z32">
-        <v>0.0002018555548184721</v>
+        <v>0.0002098280763503452</v>
       </c>
       <c r="AA32">
-        <v>1.895357322239175E-06</v>
+        <v>1.353729524840937E-05</v>
       </c>
       <c r="AB32">
-        <v>0.0001317273338956227</v>
+        <v>0.0001353729524840937</v>
       </c>
       <c r="AC32">
-        <v>9.476786611195875E-07</v>
+        <v>9.669496606006691E-07</v>
       </c>
       <c r="AD32">
         <v>0</v>
@@ -3894,10 +3894,10 @@
         <v>0</v>
       </c>
       <c r="AH32">
-        <v>0.0002340766292965381</v>
+        <v>0.0002388365661683653</v>
       </c>
       <c r="AI32">
-        <v>0.0003800191431089546</v>
+        <v>0.0003896807132220697</v>
       </c>
     </row>
     <row r="33" spans="1:35">
@@ -3914,10 +3914,10 @@
         <v>0</v>
       </c>
       <c r="E33">
-        <v>9.476786611195875E-07</v>
+        <v>9.669496606006691E-07</v>
       </c>
       <c r="F33">
-        <v>9.476786611195875E-07</v>
+        <v>9.669496606006691E-07</v>
       </c>
       <c r="G33">
         <v>0</v>
@@ -3944,13 +3944,13 @@
         <v>0</v>
       </c>
       <c r="O33">
-        <v>1.231982259455464E-05</v>
+        <v>1.25703455878087E-05</v>
       </c>
       <c r="P33">
-        <v>2.843035983358763E-06</v>
+        <v>2.900848981802008E-06</v>
       </c>
       <c r="Q33">
-        <v>9.476786611195875E-07</v>
+        <v>9.669496606006691E-07</v>
       </c>
       <c r="R33">
         <v>0</v>
@@ -3959,13 +3959,13 @@
         <v>0</v>
       </c>
       <c r="T33">
-        <v>7.5814292889567E-06</v>
+        <v>7.735597284805353E-06</v>
       </c>
       <c r="U33">
         <v>0</v>
       </c>
       <c r="V33">
-        <v>0.0007932070393570948</v>
+        <v>0.0008093368659227601</v>
       </c>
       <c r="W33">
         <v>0</v>
@@ -3974,16 +3974,16 @@
         <v>0</v>
       </c>
       <c r="Y33">
-        <v>9.476786611195875E-07</v>
+        <v>9.669496606006691E-07</v>
       </c>
       <c r="Z33">
-        <v>3.79071464447835E-06</v>
+        <v>3.867798642402676E-06</v>
       </c>
       <c r="AA33">
         <v>0</v>
       </c>
       <c r="AB33">
-        <v>2.843035983358763E-06</v>
+        <v>2.900848981802008E-06</v>
       </c>
       <c r="AC33">
         <v>0</v>
@@ -4012,88 +4012,88 @@
         <v>32</v>
       </c>
       <c r="B34">
-        <v>0.004298670406838449</v>
+        <v>0.004113403856195246</v>
       </c>
       <c r="C34">
-        <v>0</v>
+        <v>3.867798642402676E-06</v>
       </c>
       <c r="D34">
-        <v>0.0001137214393343505</v>
+        <v>0.0001208687075750836</v>
       </c>
       <c r="E34">
-        <v>0</v>
+        <v>2.320679185441606E-05</v>
       </c>
       <c r="F34">
-        <v>3.411643180030515E-05</v>
+        <v>7.445512386625153E-05</v>
       </c>
       <c r="G34">
-        <v>0.0003989727163313464</v>
+        <v>0.0004167553037188884</v>
       </c>
       <c r="H34">
-        <v>9.476786611195875E-07</v>
+        <v>1.160339592720803E-05</v>
       </c>
       <c r="I34">
         <v>0</v>
       </c>
       <c r="J34">
-        <v>2.558732385022886E-05</v>
+        <v>3.190933879982208E-05</v>
       </c>
       <c r="K34">
-        <v>1.895357322239175E-05</v>
+        <v>2.417374151501673E-05</v>
       </c>
       <c r="L34">
-        <v>9.476786611195875E-07</v>
+        <v>1.837204355141271E-05</v>
       </c>
       <c r="M34">
-        <v>9.476786611195875E-07</v>
+        <v>9.669496606006691E-07</v>
       </c>
       <c r="N34">
-        <v>4.738393305597937E-06</v>
+        <v>2.417374151501673E-05</v>
       </c>
       <c r="O34">
-        <v>2.843035983358763E-06</v>
+        <v>4.834748303003346E-06</v>
       </c>
       <c r="P34">
-        <v>4.738393305597937E-06</v>
+        <v>2.030594287261405E-05</v>
       </c>
       <c r="Q34">
-        <v>3.506411046142474E-05</v>
+        <v>5.02813823512348E-05</v>
       </c>
       <c r="R34">
-        <v>9.476786611195875E-07</v>
+        <v>1.25703455878087E-05</v>
       </c>
       <c r="S34">
-        <v>0</v>
+        <v>1.643814423021138E-05</v>
       </c>
       <c r="T34">
-        <v>9.476786611195875E-07</v>
+        <v>7.735597284805353E-06</v>
       </c>
       <c r="U34">
-        <v>3.885482510590309E-05</v>
+        <v>6.285172793904349E-05</v>
       </c>
       <c r="V34">
-        <v>0.0002141753774130268</v>
+        <v>0.0002311009688835599</v>
       </c>
       <c r="W34">
-        <v>0</v>
+        <v>2.900848981802008E-06</v>
       </c>
       <c r="X34">
-        <v>0</v>
+        <v>1.933899321201338E-06</v>
       </c>
       <c r="Y34">
-        <v>0</v>
+        <v>7.735597284805353E-06</v>
       </c>
       <c r="Z34">
-        <v>0</v>
+        <v>9.669496606006691E-07</v>
       </c>
       <c r="AA34">
-        <v>7.960500753404536E-05</v>
+        <v>9.379411707826491E-05</v>
       </c>
       <c r="AB34">
-        <v>0</v>
+        <v>1.933899321201338E-06</v>
       </c>
       <c r="AC34">
-        <v>0.0002340766292965381</v>
+        <v>0.0002388365661683653</v>
       </c>
       <c r="AD34">
         <v>0</v>
@@ -4105,13 +4105,13 @@
         <v>0</v>
       </c>
       <c r="AG34">
-        <v>0</v>
+        <v>1.933899321201338E-06</v>
       </c>
       <c r="AH34">
-        <v>3.222107447806598E-05</v>
+        <v>3.287628846042275E-05</v>
       </c>
       <c r="AI34">
-        <v>9.476786611195875E-07</v>
+        <v>1.933899321201338E-06</v>
       </c>
     </row>
     <row r="35" spans="1:35">
@@ -4119,88 +4119,88 @@
         <v>33</v>
       </c>
       <c r="B35">
-        <v>0.009133726935870584</v>
+        <v>0.008770233421648069</v>
       </c>
       <c r="C35">
-        <v>4.738393305597937E-06</v>
+        <v>1.160339592720803E-05</v>
       </c>
       <c r="D35">
-        <v>2.937803849470721E-05</v>
+        <v>4.544663404823145E-05</v>
       </c>
       <c r="E35">
-        <v>0.0001942741255295154</v>
+        <v>0.0002446382641319693</v>
       </c>
       <c r="F35">
-        <v>3.222107447806598E-05</v>
+        <v>8.799241911466088E-05</v>
       </c>
       <c r="G35">
-        <v>0.000124145904606666</v>
+        <v>0.0001595466939991104</v>
       </c>
       <c r="H35">
-        <v>6.633750627837113E-05</v>
+        <v>8.12237714904562E-05</v>
       </c>
       <c r="I35">
         <v>0</v>
       </c>
       <c r="J35">
-        <v>7.202357824508865E-05</v>
+        <v>8.509157013285888E-05</v>
       </c>
       <c r="K35">
-        <v>0.0001866926962405587</v>
+        <v>0.0002117619756715465</v>
       </c>
       <c r="L35">
-        <v>1.51628585779134E-05</v>
+        <v>4.641358370883212E-05</v>
       </c>
       <c r="M35">
-        <v>0.0001070876887065134</v>
+        <v>0.0001092653116478756</v>
       </c>
       <c r="N35">
-        <v>0.0002473441305522124</v>
+        <v>0.0002736467539499894</v>
       </c>
       <c r="O35">
-        <v>0.0007259218544176041</v>
+        <v>0.0007445512386625152</v>
       </c>
       <c r="P35">
-        <v>0.0004046587882980639</v>
+        <v>0.0004312595486278985</v>
       </c>
       <c r="Q35">
-        <v>0.001015911524720198</v>
+        <v>0.001074281072927343</v>
       </c>
       <c r="R35">
-        <v>2.843035983358763E-06</v>
+        <v>3.674408710282543E-05</v>
       </c>
       <c r="S35">
-        <v>9.476786611195875E-07</v>
+        <v>6.57525769208455E-05</v>
       </c>
       <c r="T35">
-        <v>2.27442878668701E-05</v>
+        <v>2.900848981802007E-05</v>
       </c>
       <c r="U35">
-        <v>0.0001592100150680907</v>
+        <v>0.0002282001199017579</v>
       </c>
       <c r="V35">
-        <v>0.001727618199221008</v>
+        <v>0.00177822042584463</v>
       </c>
       <c r="W35">
-        <v>0</v>
+        <v>1.643814423021138E-05</v>
       </c>
       <c r="X35">
-        <v>9.476786611195875E-07</v>
+        <v>1.933899321201338E-06</v>
       </c>
       <c r="Y35">
-        <v>0.000103296974062035</v>
+        <v>0.000114100059950879</v>
       </c>
       <c r="Z35">
-        <v>0.000108035367367633</v>
+        <v>0.0001150670096114796</v>
       </c>
       <c r="AA35">
-        <v>0.0002407103799243752</v>
+        <v>0.00026010945870158</v>
       </c>
       <c r="AB35">
-        <v>4.738393305597937E-06</v>
+        <v>4.834748303003346E-06</v>
       </c>
       <c r="AC35">
-        <v>0.0006927531012784185</v>
+        <v>0.0007068402018990892</v>
       </c>
       <c r="AD35">
         <v>0</v>
@@ -4212,13 +4212,13 @@
         <v>0</v>
       </c>
       <c r="AG35">
-        <v>0</v>
+        <v>1.933899321201338E-06</v>
       </c>
       <c r="AH35">
-        <v>6.538982761725154E-05</v>
+        <v>6.671952658144617E-05</v>
       </c>
       <c r="AI35">
-        <v>2.748268117246804E-05</v>
+        <v>2.900848981802007E-05</v>
       </c>
     </row>
   </sheetData>

</xml_diff>